<commit_message>
Añadidas fuentes de descripciones
</commit_message>
<xml_diff>
--- a/Datos/Datos IEET/Scraping Inventario/Descripciones Mamíferos.xlsx
+++ b/Datos/Datos IEET/Scraping Inventario/Descripciones Mamíferos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Description</t>
         </is>
       </c>
@@ -453,6 +458,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>“Ammotragus” significa “cabra de las arenas” y su aspecto general es el de una cabra robusta, de faz alargada y extremidades relativamente cortas y macizas, destacando así mismo una cola relativamente larga. Medidas corporales, CC: 105-176 cm (machos), 104-150 cm (hembras); CR: 90-100 cm (machos), 75-90 cm (hembras); Ps: 50-132 kg (machos), 12-68 kg (hembras). Predomina un tono pálido leonado. La característica más notable es su larga melena que se extiende desde la garganta hasta el pecho, a partir del cual se bifurca y continúa por las patas delanteras. No posee barba de chivo y, al igual que las ovejas, poseen barba en las mejillas y una crin en el dorso. Los cuernos, con una sola inflexión, forman una circunferencia hacia arriba y atrás, y en machos maduros la parte distal va convergiendo por encima de la nuca. Carece de glándulas preorbitales, interdigitales y laterales, aunque sí posee glándulas subcaudales. Las hembras poseen un solo par de mamas inguinales. Fórmula dentaria: 0.0.3.3/3.1.3.3. Número de cromosomas (2n) = 58.</t>
         </is>
       </c>
@@ -465,6 +475,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>De mayor tamaño que A. sylvaticus. Los adultos presentan una coloración dorsal pardo rojiza, clara y brillante, que se diferencia netamente de la coloración blanca del vientre. Suele presentar una mancha pectoral en forma de collar más o menos grande y completa, aunque no se trata de una característica determinante. Medidas corporales, CC: 86,0-120,0 mm; C: 100,0-130,0 mm (entre 170 y 230 anillos); P: 22,0-25,0 mm; O: 16,0-19,0 mm; Ps: 20,0-50,0 g. No existe dimorfismo sexual. Las hembras presentan tres pares de mamas: uno pectoral y dos inguinales. Los individuos juveniles y subadultos, mucho mas oscuros, son muy difíciles de distinguir de A. sylvaticus, sin embargo, la confusión con los ratones del género Mus es imposible pues la longitud del pie es siempre superior a 20 mm. Fórmula dentaria: 1.0.0.3/1.0.0.3. Ausencia del tubérculo 9 del M2 y con un tubérculo 7 bien desarrollado en el M1. Número de cromosomas (2n) = 48 (en Bulgaria se ha descrito una forma con 49).</t>
         </is>
       </c>
@@ -477,6 +492,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Es un múrido de tamaño relativamente pequeño y aspecto grácil. Medidas corporales, CC: 73,0-101,5 mm; C: 68,0-98,5 mm; P: 15,5-17,5 mm; O: 11,5-15,0 mm; Ps: 12,5-29,0 g. La longitud de la cola es similar a la de la cabeza y cuerpo (carácter diferencial respecto al ratón moruno Mus spretus, en el que la cola nunca supera dicha longitud) y recubierta de escamas entre las que se disponen de forma dispersa pelos cortos y finos. El hocico es ligeramente alargado y puntiagudo, los ojos negros y pequeños y las orejas redondeadas. El color del pelaje es variable. Los juveniles presentan una coloración uniforme gris oscura que desaparece tras el primer cambio de pelaje. En subadultos y adultos existe una amplia gama entre dos tipos de coloraciones extremas, la clara y la oscura. Las formas claras presentan el dorso y la cola pardo-grisácea y la región ventral y las extremidades de crema a blanco, ligeramente lavado de gris, con una línea clara de demarcación entre ambas regiones. Los animales de coloración oscura tienen el dorso, cola y patas de color gris parduzco oscuro, y el vientre ligeramente más claro, sin línea neta de demarcación. En los animales comensales predomina la coloración oscura y en las formas asilvestradas la coloración clara, aunque en una misma población pueden aparecer todas las variaciones posibles. Las hembras presentan cinco pares de mamas, tres pectorales y dos inguinales. El cráneo es pequeño, anguloso y de perfil ligeramente convexo. La placa zigomática, de perfil anterior rectilíneo, presenta un foramen que está ausente en M. spretus. La rama dorsal del arco zigomático es estrecha. La mandíbula se distingue de la del ratón de campo Apodemus sylvaticus, por presentar la escotadura entre las apófisis angular y articular en forma de media luna. Fórmula dentaria: 1.0.0.3/1.0.0.3. Los molares son bunodontos, de crecimiento limitado y con raíces cerradas. Los incisivos superiores presentan la cara externa redondeada con una ligera pigmentación anaranjada. La parte anterior del M1 es trilobulada, a diferencia de M. spretus, que tiene cuatro tubérculos. Número estándar de cromosomas (2n) = 40, con 19 pares de cromosomas autosómicos ( todos ellos acrocéntricos) y la pareja de cromosomas sexuales. 461 Catalán: Ratolí domèstic l Eusquera: Etxe-sagua l Gallego: Rato caseiro Alemán: Westliche hausmaus l Francés: Souris domestique l Inglés: House mouse l Portugués: Rato-caseiro Orden Rodentia l  Suborden Myomorpha l  Familia Muridae l  Subfamilia Murinae ESPECIE AUTÓCTONA Ratón casero Mus musculus Linnaeus, 1758</t>
         </is>
       </c>
@@ -489,6 +509,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>La rata de agua es un arvicolino de tamaño medio, CC: 170,0-230,0 mm; C: 100,0-147,0 mm; P: 32,0-39,0 mm; O: 12,0-22,0 mm; Ps: 140,0-310,0 g. En comparación con la rata topera (Arvicola terrestris) de la Península Ibérico, su aspecto general es más robusto, su tamaño corporal significativamente mayor y su cola relativamente más larga, superando siempre la mitad de la longitud de la cabeza más el cuerpo. No existe dimorfismo sexual a escala somática y craneal, si bien durante la etapa adulta los machos adultos tienden a ser, por término medio, algo mayores que las hembras. En ambos sexos existe en cada flanco una glándula odorífera cutánea de forma ovalada. Se distinguen dos patrones de coloración del pelaje que se utilizan como criterio básico para la diagnosis subespecífica. De manera general, en los adultos de la subespecie nominal el dorso varía desde pardo amarillento hasta pardo oscuro salpicado de negro. Los flancos son ligeramente más claros que la parte dorsal debido al predominio de tonalidades ocráceas. El vientre es gris ceniza mezclado de amarillo en intensidad variable; la parte más anterior del pecho y la garganta son algo más claras debido a la mayor abundancia de pelos blanquecinos. La cola es bicolor, pardo oscura por encima y más clara ventralmente. El pelaje juvenil es en conjunto más oscuro que el de los adultos. Respecto a la subespecie nominal, A. s. tenebricus muestra una coloración general más oscura, existiendo una conspicua profusión de pelos negros en los flancos y cara. Presentan tres pares de mamas, uno pectoral y dos inguinales. El cráneo adulto es robusto, anguloso y muy plano dorsalmente. Los incisivos superiores son ortodontos (compárese con A. terrestris) y los molares hipsodontos y sin raíces. Fórmula dentaria: 1.0.0.3/1.0.0.3. Los huesos nasales son en su tercio anterior casi iguales de ancho que el rostro, la apófisis articular de la man405 Catalán: Rata d’aigua l Eusquera: Mendebaldeko ur-arratoia l Gallego: Rata de auga común Alemán: Südwesteuropäische Schermaus l Francés: Campagnol amphibie l Inglés: Southern water vole l Portugués: Rato-de-água  Orden Rodentia l  Suborden Myomorpha l  Familia Cricetidae l  Subfamilia Arvicolinae ESPECIE AUTÓCTONA Rata de agua Arvicola sapidus Miller, 1908 díbula es relativamente plana en su cara externa y está marcadamente separada de la apófisis angular, y el bucle anterior del M1 está ligeramente aplanado en su parte anterior y forma un ángulo agudo en la parte lingual (compárese con A. terrestris). Número de cromosomas (2n) = 40.</t>
         </is>
       </c>
@@ -501,6 +526,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>La especie muestra una gran variabilidad morfológica a lo largo de su extensa área de distribución. En la Península Ibérica A. terrestris está representada por morfotipos de pequeño tamaño, CC: 122,0188,0 mm; C: 49,0-85,5 mm; P: 22,0-27,5 mm; O: 10,0-14,5 mm; Ps: 66,0-183,0 g, correspondientes a la forma cavadora. Sus dimensiones corporales son sensiblemente menores que las de la rata de agua, Arvicola sapidus, y su cola relativamente más corta (su longitud es siempre inferior a la mitad de la longitud de la cabeza más el cuerpo). En lo referente a las medidas somáticas y craneales no cabe hablar, en términos generales, de dimorfismo sexual. Machos y hembras muestran un par de glándulas odoríferas cutáneas situadas a ambos flancos del cuerpo y cuyo tejido secretor alcanza su mayor desarrollo en los adultos durante el período reproductor. La coloración del pelaje es muy variable existiendo conspicuas diferencias incluso a escala intrapoblacional. En los ejemplares del Valle de Arán (Lleida) el dorso varía desde pardo oscuro o pardo amarillento hasta gris ceniza y los flancos desde pardo amarillento u ocre hasta gris claro; en la región ventral predominan los tonos grisáceos, ya sea mezclados con amarillo, ocre o negro o bien profusamente lavados de blanco. La cola es generalmente bicolor, con la zona dorsal de tonos semejantes a la región mediodorsal del cuerpo y la parte ventral algo más clara. Los juveniles poseen un pelaje más oscuro que los adultos, pardusco en el dorso y 401 Catalán: Rata talpera l Eusquera: Ekialdeko ur-arratoia l Gallego: Rata de auga norteña Alemán: Schermaus l Francés: Campagnol terrestre l Inglés: Water vole l Portugués: Rato-dos-lameiros Orden Rodentia l  Suborden Myomorpha l  Familia Cricetidae l  Subfamilia Arvicolinae ESPECIE AUTÓCTONA Rata topera Arvicola terrestris (Linnaeus, 1758) gris ceniza en la región ventral. Presenta cuatro pares de mamas, dos pectorales y dos inguinales. El cráneo es compacto y anguloso, especialmente en los adultos. Los molares son hipsodontos y sin raíces. Fórmula dentaria: 1.0.0.3/1.0.0.3. Por el cráneo y la dentición se diferencia de A. sapidus por los siguientes caracteres: los huesos nasales son en su tercio anterior claramente más estrechos que el rostro; en la mandíbula, la apófisis angular se encuentra muy próxima a la base de la rama articular; los incisivos superiores son prodontos; el bucle anterior del M1 es redondeado en su parte anterior y forma un ángulo obtuso en la parte lingual. Número de cromosomas (2n) = 36.</t>
         </is>
       </c>
@@ -513,6 +543,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>Algo más pequeño que los otros erizos europeos (Erinaceus europaeus y Erinaceus concolor). En las Baleares y la Península Ibérica los adultos de mayor edad presentan un pelaje blanquecino, con la cara, las extremidades y, a veces, la zona genital algo oscurecidas. Los ejemplares juveniles presentan un pelaje parcialmente pardo oscuro, principalmente en su parte ventral posterior. Las púas de los ejemplares adultos son de color muy claro, con un anillo oscuro hacia la mitad, algo más cercano a la raíz que al ápice. Las púas de la cabeza se hallan separadas por una franja central relativamente ancha. El pulgar del pie posterior es pequeño, sin que su ápice alcance la base del segundo dedo. Las callosidades de los pies son características. El borde posterior del paladar es ancho y engloba a la espina media posterior. Las bullas timpánicas están reducidas. El PM2 carece de cúspide lingual. Medidas corporales de ejemplares adultos de Mallorca, CC: 194,0-245,0 mm; C: 20,0-40,0 mm; P: 36,0-42,0 mm; Ps: 280,0-657,0 g. Fórmula dentaria: 3.1.3.3/2.1.2.3. Número de cromosomas (2n) = 48.</t>
         </is>
       </c>
@@ -525,6 +560,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Se trata de una ardilla terrestre cuyo aspecto es muy semejante al de la mayoría de las ardillas de suelo. Su cuerpo y cola están recorridos longitudinalmente por cuatro bandas negras y dos blancas. El pelo es corto, salvo la cola que es muy poblada, de pelo largo y denso, y con bandas longitudinales de colores pardo y oscuro. La cabeza de color pardo-rojiza resulta proporcionalmente grande en relación al resto del cuerpo. El hocico es oscuro y las mandíbulas casi blancas, mientras que las orejas son pequeñas, casi inexistentes, y no poseen penachos. Las hembras presentan cuatro pares de mamas que se reparten desde la zona genital hasta cubrir las tres cuartas partes de la distancia entre las extremidades posteriores y las anteriores. Los machos son algo mayores que las hembras, CC: 170,0-200,0 mm; C: 130,0 -140,0 mm; P: 45,0-48,0 mm; Ps: 232,0-280,0 g (machos), 209,0-250,0 g (hembras). Fórmula dentaria: 1.0.2.3/1.0.1.3. Número de cromosomas (2n) = 38.</t>
         </is>
       </c>
@@ -537,6 +577,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Murciélago de talla media. Destacan sus orejas grandes de forma cuadrangular, unidas en la frente en su borde interno y con un pequeño lóbulo saliente en el externo, aunque no siempre está presente. La coloración del pelaje suele ser bastante oscura, entre negruzca y parda. Salvo en los ejemplares de Canarias las puntas de los pelos pueden ser en algunos casos blanquecinas. La zona ventral es también oscura aclarándose hacia la parte inguinal. ANT: 35,0-42,5 mm; Ps: 5,6-13,7 g. Las hembras son ligeramente mayores que los machos. Fórmula dentaria: 2.1.2.3/3.1.2.3. Número de cromosomas (2n) = 32. En general su aspecto, muy característico, hace que sea una especie inconfundible en España.</t>
         </is>
       </c>
@@ -549,6 +594,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>Con el aspecto de un perro pastor alemán, el lobo ibérico tiene la cabeza más grande y redondeada, con maseteros muy desarrollados, orejas cortas y triangulares, cuello robusto y grupa ligeramente hundida. Color gris parduzco, con el pelo del cuello, del dorso y de la cola gris oscuro. Tiene las mejillas blancas y una línea oscura en las patas anteriores que a veces llega hasta el pecho. Los machos son ligeramente mayores que las hembras pero el dimorfismo apenas es apreciable. Medidas corporales, CC: 120 cm; C: 40 cm; CR: 70-80 cm; Ps: 32 kg (machos), 28 kg (hembras), con máximos comprobados de 46 kg y 38 kg respectivamente. Fórmula dentaria: 3.1.4.2/3.1.4.3. Numero de cromosomas (2n) = 78.</t>
         </is>
       </c>
@@ -561,6 +611,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>Es un ungulado robusto y de mediano tamaño, CC: 97-148 cm; CR: 65-84 cm; Ps: 31-90 kg. Ambos sexos presentan cuernos persistentes, formados por un soporte óseo recubierto de un estuche córneo, no ramificados, gruesos y nudosos, que en los machos adultos se curva en forma de “S”. El número de nudos, o medrones, da una idea de la edad. Los cuernos de las hembras son más cortos, cilíndricos y en forma de lira. Los machos son mayores que las hembras y además presentan una crin y barbas características, y manchas negras en el pelaje más extensas. Las de las poblaciones del sur peninsular son más pequeñas que las del norte. El color del pelaje varía estacionalmente, presentando un pelo de color canela en verano, que se torna más oscuro en el invierno. Fórmula dentaria: 0.0.3.3/3.1.3.3. Número de cromosomas (2n) = 60.</t>
         </is>
       </c>
@@ -573,6 +628,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>Es el más pequeño de los cérvidos europeos. Los machos son de mayor tamaño que las hembras, pero el grado de dimorfismo sexual es relativamente bajo. Medidas corporales, CC: 95-145 cm; CR: 54-83 cm; Ps: 16-30 kg. Presentan unas extremidades traseras potentes, adaptadas al salto. Destacan en su morfología una franja negra en el hocico, grandes orejas, un escudo anal blanco con pelo erizable que rodea la rudimentaria cola, y astas con tres puntas y abundante “perlado” en los machos, que se renuevan anualmente. Tiene dos mudas al año, en primavera y en otoño; el manto de invierno es tupido y de color gris, y el de verano corto con gran variedad de tonalidades desde el anaranjado al castaño, si bien hay poblaciones en el sur de España que conservan la coloración gris también en verano. Fórmula dentaria: 0.0.3.3./3.1.3.3. Número de cromosomas (2n) = 70.</t>
         </is>
       </c>
@@ -585,6 +645,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>Pelaje con predominio del color castaño uniforme, zona ventral más clara y escudo anal casi blanco flanqueado por bandas oscuras en ocasiones casi negras, cola corta de color oscuro. Los cervatillos tienen un pelaje característico con fondo castaño y manchas o “pintas” blancas que mantienen durante aproximadamente los tres primeros meses de vida. Dimorfismo sexual acentuado. Medidas corporales, CC: 160-220 cm (machos), 160-195 cm (hembras); CR: 90-120 cm (machos), 90-110 cm (hembras); Ps: 80-160 kg (machos), 50-100 kg (hembras). Los machos desarrollan a partir del primer año unas astas que utilizan en las luchas durante el período de celo. Presentan un tronco central que se ramifica en puntas o candiles en número variable. Las hembras carecen de astas y poseen dos pares de mamas en posición inguinal. Fórmula dentaria: 0.1.3.3/3.1.3.3, con un canino inferior modificado hasta adoptar forma de incisivo. Número de cromosomas (2n) = 68.</t>
         </is>
       </c>
@@ -597,6 +662,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>Es uno de los arvicolinos ibéricos de mayor tamaño. Medidas corporales de ejemplares de Cataluña, CC: 92,0-140,0 mm; C: 45,0-74,0 mm; P: 17,5-25,0 mm; O: 12,5-21,0 mm; Ps: 35,0-70,0 g. El pelaje presenta una tonalidad bastante uniforme de color grisáceo y con tonos pardos. En juveniles y subadultos no presenta tonos pardos y es más claro. La región ventral es de color blanco, a veces con tonos grisáceos claros. Los pies y la cola son monocolor, generalmente blanquecinos. En comparación con los otros topillos ibéricos, la cola de Ch. nivalis es proporcionalmente más larga, con una longitud cercana o superior al 50% de la longitud de la cabeza más el cuerpo. Otro carácter externo significativo es la gran longitud de sus vibrisas. Estas características morfológicas ponen de manifiesto la naturaleza rupícola de Ch. nivalis. Presenta cuatro pares de mamas, dos pectorales y dos inguinales. Cráneo alargado con una ligera depresión a nivel de los huesos frontales. Dientes de crecimiento continuo y raíz abierta. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 54.</t>
         </is>
       </c>
@@ -609,6 +679,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>Es un crocidurino de talla media. Medidas corporales, CC: 54,0-74,0 mm; C: 31,0-47,5 mm; P: 12,014,4 mm; Ps: 6,0-9,5 g, de orejas largas y pelaje largo y suave que mantiene todo el año. El pelaje dorsal es de color pardogrisáceo oscuro, mientras que el ventral, también de tonalidad oscura, presenta en la punta de sus pelos una coloración blancuzca o beige que junto al gris oscuro de su base le confiere un aspecto jaspeado. La cola, las orejas y las extremidades son de color más claro y están cubiertas por pelos finos blancuzcos. Las hembras presentan tres pares de mamas en posición inguinal. En comparación con C. russula, posee una caja craneana levemente más redondeada, y las regiones rostral, maxilar e interorbital son más esbeltas. En vista lateral, el cráneo es largo y presenta un perfil dorsal más abombado. Fórmula dentaria: 3.1.1.3/1.1.1.3. El tamaño de los tres unicúspides superiores es mayor que en C. russula. Además, el paracono del cuarto premolar es pequeño y está completamente unido al metacono. La superficie posterior del proceso condilar tiene forma de L. Número de cromosomas (2n) = 36.</t>
         </is>
       </c>
@@ -621,6 +696,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>Es un crocidurino de talla mediana. Medidas corporales, CC: 62,0-84,0 mm; C: 34,0-47,0 mm; P: 11,0-14,0 mm; Ps: 7,0-14,0 g, y cola relativamente corta, recubierta por pelos cortos entre los que sobresalen otros más largos y dispersos. Los ojos son pequeños y los pabellones auditivos están bien desarrollados y son visibles externamente. El color del pelaje varía en función de la edad, la época del año y la localización geográfica. En general, la coloración es gris uniforme en los juveniles, parda o pardagrisácea en los ejemplares de verano y gris oscura en los de invierno. El vientre es gris claro, sin demarcación nítida respecto al dorso. Presenta tres pares de mamas inguinales. El cráneo es más largo y macizo que en los representantes del género Sorex. Las regiones rostral e interorbital son alargadas y el margen posterior del orificio nasal es cóncavo. La caja craneana es alta y los cóndilos occipitales están proyectados hacia atrás. La mandíbula es robusta, con el cóndilo articular bien desarrollado y la apófisis coronoides recta, de altura generalmente superior a 4,2 mm. Fórmula dentaria: 3.1.1.3/1.1.1.3, con tres unicúspides superiores. A diferencia de la musaraña de campo, Crocidura suaveolens, en visión lateral el segundo y tercer unicúspides son de talla similar y sobrepasan la altura del parastilo del cuarto molar. En visión oclusal, el protocono de este molar no está desplazado en dirección bucal y contribuye a formar el margen ántero-interno del diente. En la mandíbula, el segundo molar presenta una constricción bien marcada. Número de cromosomas (2n) = 42.</t>
         </is>
       </c>
@@ -633,6 +713,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>Es un sorícido de dientes blancos semejante a la musaraña gris, Crocidura russula. Coloración dorsal acastañada, ventralmente grisácea a veces con cierto tinte amarillento. Se ha señalado albinismo. La muda primaveral se inicia en abril, la otoñal acontece en septiembre-octubre. Como en C. russula la cola presenta unos característicos pelos largos. Posee    glándulas en los costados. En Europa continental y en la Península Ibérica las dimensiones aumentan de norte a sur. La población de Menorca es la que presenta un mayor tamaño. Medidas corporales, CC: 68,3 mm, C: 42,8 mm, P: 11,6 mm, O: 8,1 mm (País Vasco); CC: 64,3 mm, C: 42,6 mm, P: 11,6 mm, O: 7,5 mm (Asturias); CC: 62,9 mm, C: 41,8 mm, P: 11,3 mm, O: 7,1 mm (Galicia); CC: 56,2 mm, C: 37,3 mm, P: 10,7 mm, O: 7,6 mm (Andalucía); CC: 67,5 mm, C: 57,7 mm, P: 12,8 mm, O: 8,1 mm (Menorca); Ps: 5,7-8,1 g (Península Ibérica), Ps: 6,0-11,0 g (Menorca). Puede confundirse con C. russula y precisa de una detallada observación de las características dentarias para su correcta identificación. Fórmula dentaria: 3.1.1.3/1.1.1.3. Número de cromosomas (2n) = 40.</t>
         </is>
       </c>
@@ -645,6 +730,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>Sorícido de tamaño reducido, de cabeza voluminosa y orejas grandes. Antitrago muy grande y redondeado, provisto de una franja de pelos largos. Presenta largas vibrisas faciales. Posee una cola no demasiado larga. El pelaje del cuerpo es corto y suave, de color gris claro en el dorso y blanco en el vientre y en los pies. Son frecuentes los ejemplares albinos. Medidas corporales, CC: 53,0-64,0 mm; C: 27,0-39,0 mm; P: 10,0-13,0 mm; O: 7,0-11,0 mm. Presenta tres pares de mamas inguinales. Fórmula dentaria: 3.1.1.3/1.1.1.3.</t>
         </is>
       </c>
@@ -657,6 +747,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>Los machos exhiben una cornamenta aplanada, de forma muy diferente a la del resto de los representantes de la familia, y que solamente presentaban los fósiles Dama clactoniana y Megaceros. El gamo tiene dos pelajes o libreas, una en verano y otra en invierno. En general, el color de la época estival posee un fondo cervuno ligeramente rojizo, moteado de manchas blancas. En ambos flancos, cuando se aproximan a la zona ventral, dichas manchas se van alargando y tienden generalmente a unirse entre ellas para terminar formando una banda longitudinal blanca. Asimismo, a lo largo del dorso aparece una lista sepia que se va oscureciendo según se acerca a la cola. La cabeza suele carecer de manchas. El vientre y la cara interior de sus miembros son blancos. En invierno la coloración se torna más oscura y las manchas blancas desaparecen por completo. Posee uno de los escudos anales más elaborados de entre los cérvidos, consistente en una gran mancha blanca que está limitada a cada lado por una línea vertical negra y dividida por la porción superior negra de la cola, la cual es blanca en su cara ventral. Entre los gamos, el dimorfismo sexual es muy acentuado. Sólo los machos presentan astas que, echadas hacia atrás e implantadas sobre pedúnculos muy cortos, presentan tres candiles y una ancha palma, característica de la especie. La cornamenta sufre mudas anuales durante toda la vida del animal, cayendo normalmente a finales del invierno para volver a crecer en primavera cubierta de un terciopelo que se va desprendiendo durante el verano. Medidas corporales de ejemplares adultos de Doñana, CC: 129155 cm (machos), 118-140 cm (hembras); CR: 85 cm (machos), 75 cm (hembras); Ps: 52-63 kg (machos), 28-41 kg (hembras). Fórmula dentaria: 0.0.3.3/3.1.3.3. Número de cromosomas (2n) = 68.</t>
         </is>
       </c>
@@ -669,6 +764,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>Es un mamífero de pequeño tamaño, de aspecto rechoncho, cabeza voluminosa y hocico muy prolongado en forma de trompa cilíndrica ligeramente comprimida, con un surco a lo largo de su cara inferior y terminado en un pequeño rinario hendido verticalmente en el centro. Orejas grandes y anchas. Extremidades pentadáctilas con palmas y plantas desnudas, las posteriores  son muy largas y estrechas. La cola es algo más larga que el cuerpo, presentando en su cara inferior, a dos centímetros de la base, una glándula odorífera. Pelaje espeso y blando, de color pardo madera en el dorso y blanco en la superficie ventral y en los cuatro pies. Presentan cierto dimorfismo sexual. Medidas corporales, CC: 100,0110,0 mm; C: 106,0-120,0 mm; O: 24,0-25,0 mm; P: 31,0-35,0 mm. Fórmula dentaria: 3.1.4.2/3.1.4.2. Número de cromosomas (2n) = 28. Las hembras poseen de dos a tres pares de mamas.</t>
         </is>
       </c>
@@ -681,6 +781,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>Debe su nombre a una franja de pelo negro que, como un antifaz, le enmarca los ojos y le cubre parte de la cara. Su aspecto es inconfundible, aunque sus hábitos trepadores y su color rojizo pueden asemejarle al lirón gris Glis glis, o a la ardilla roja Sciurus vulgaris. Los adultos presentan el dorso pardorojizo y el vientre blanco. La cola es larga y está cubierta de pelos, con un llamativo pincel de pelo largo blanco y negro en el extremo. Hocico alargado y orejas grandes. No presentan dimorfismo sexual. Las hembras presentan cuatro pares de mamas: uno pectoral, otro abdominal y dos pares inguinales. Medidas corporales, CC: 118,0-136,0 mm; C: 98,5-113,0 mm; P: 26,5-28,5 mm; Ps: 45,0-120,0 g. Se producen variaciones estacionales en el peso debido al carácter hibernante de la especie. El cráneo es de aspecto macizo y de perfil dorsal convexo. La caja craneana es cuadrada, el rostro largo, los huesos nasales muy estrechos en la parte posterior y los arcos zigomáticos amplios. Las bullas timpánicas presentan gran desarrollo, carácter típico de las especies de roedores de climas desérticos, con densidades de población escasas. Fórmula dentaria: 1.0.1.3/1.0.1.3. Es el único roedor español cuya mandíbula presenta un orificio natural en la apófisis angular, lo que facilita su identificación en los análisis de egagrópilas, excrementos, etc. Número de cromosomas (2n) = 46-52.</t>
         </is>
       </c>
@@ -693,6 +798,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>Murciélago de talla grande. Pelo monocolor, a veces con la punta lustrosa. Dorso pardo oscuro en E.serotinus y pálido llegando a amarillento en E.isabellinus. Vientre más claro. Los jóvenes de color grisáceo. Orejas triangulares y cortas, trago lineal con extremo redondeado. Inserción de las membranas alares en la base de los pies. Lóbulo poscalcáneo patente. ANT: 46,0-55,0 mm; Ps: 17,0-28,0 g. Las hembras son mayores que los machos. Fórmula dentaria: 2.1.1.3/3.1.2.3. Incisivos superiores externos monocúspides e internos bífidos. Número de cromosomas (2n) = 50. Entre las especies similares, el nóctulo mediano tiene el trago arriñonado, incisivos superiores externos bífidos y los internos monocúspides.</t>
         </is>
       </c>
@@ -705,6 +815,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>El aspecto general de los erizos es fácilmente reconocible por su zona dorsal recubierta de espinas, a excepción del rostro. El pelaje ventral es cerdoso, de color pardo, más o menos oscuro, según los individuos, pero con el vientre blancuzco. Ambos sexos son parecidos, ya que los testículos son intraabdominales. La principal diferencia consiste en que el pene está bastante adelantado, mientras que la vagina se localiza cerca del ano. Las hembras presentan cinco pares de mamas, una pectoral, dos abdominales y dos inguinales. Fórmula dentaria: 3.1.3.3/2.1.2.3. Sólo puede confundirse con el erizo moruno, Atelerix algirus, menos robusto, más claro, con las orejas proporcionalmente mayores y con las púas cefálicas más retrasadas. Las principales diferencias dentarias consisten en que el I3 es generalmente monoradiculado en E. europaeus y biradiculado en A. Algirus. El PM2 tiene un paracónido destacado netamente, ligeramente menor que el protocónido, mientras que en A. algirus es mucho más pequeño. Medidas corporales, CC: 190,0-290,0 mm; C: 22,0-40,0 mm; P: 46,0-53,0 mm; O: 25,029,0 mm ; Ps: 500,0-1.200,0 g. Número de cromosomas (2n) = 48.</t>
         </is>
       </c>
@@ -717,6 +832,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>Tamaño corporal y proporciones similares a las del gato montés europeo, Felis silvestris. La longitud de la cola es aproximadamente la mitad que la del cuerpo. Pelaje dorsal de color arena, con dos a cuatro líneas longitudinales oscuras en el cuello, dorso de las orejas de color rojizo con el ápice oscuro, y en algunos ejemplares rayas o manchas apenas marcadas en los flancos. Cola que disminuye de grosor hacia el extremo, con dos o más anillos oscuros y el extremo negro. Fórmula dentaria: 3.1.3.1/3.1.2.1. Medidas corporales de individuos de Marruecos, CC: 50,0-73,0 cm (machos), 45,060,0 cm (hembras); C: 25,0-33,0 cm (machos), 21,0-38,0 cm (hembras); Ps: 3,7-6,5 kg (machos), 3,05,5 kg (hembras). Número de cromosomas (2n) = 38. Los individuos de gato montés africano pueden confundirse con gatos domésticos de fenotipo “tabby”. El índice craneométrico utilizado para diferenciar F. silvestris y F. catus no es efectivo al comparar este último con F. libyca.</t>
         </is>
       </c>
@@ -729,6 +849,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>Cuerpo largo con extremidades cortas. Longitud de la cola algo mayor que la mitad de la del cuerpo. Pelaje dorsal de color gris parduzco, con cuatro o cinco líneas longitudinales negras en el cuello, una banda espinal negra y diversas bandas transversales pardas en los flancos. Ventralmente blanquecino en garganta y cuello, y de color ante-crema en el resto. Cola cilíndrica con dos o tres anillos oscuros y extremo negro. Manos con cinco dedos y pies con cuatro, todos con uñas retráctiles. Fórmula dentaria: 3.1.3.1/3.1.2.1. Cuatro pares de mamas. Dimorfismo sexual (machos mayores y más pesados que las hembras) patente desde el desarrollo juvenil. Medidas externas correspondientes a gatos adultos de Francia, CC: 52,0-65,0 cm (machos), 48,5-57,0 cm (hembras); C: 26,0-34,5 cm (machos), 25,0-32,0 cm (hembras); P: 12,0-15,0 cm (machos), 11,5-13,5 cm (hembras); Ps: 3,4-7,5 kg (machos), 3,0-5,0 kg (hembras). Número de cromosomas (2n) = 38. Los individuos vivos de F. silvestris pueden confundirse externamente con gatos cimarrones (Felis catus) de tipo “tabby”, pero se pueden identificar mediante análisis genético. Se ha descrito un método osteométrico para distinguir los cráneos.</t>
         </is>
       </c>
@@ -741,6 +866,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>Es un animal inconfundible. Su trompa, aplastada y desnuda, destaca de un cuerpo rechoncho, con una gruesa cola escamosa, de sección redondeada, pero comprimida lateralmente en su extremo. Ojos muy pequeños y ausencia de pabellones auditivos. Pelo largo y liso de color castaño o gris, con irisaciones y el vientre más claro. Extremidades posteriores mucho mayores que las anteriores y adaptadas a la natación, con membranas interdigitales. Cráneo similar al de los topos, en el que destacan los I1 de gran tamaño y forma triangular. Apófisis coronoides de la mandíbula mucho más elevada que la de los topos. Medidas corporales, CC: 115,0-135,0 mm; C: 125,0-160,0 mm; P: 27,0-34,0 mm; Ps: 50,076,0 g. Fórmula dentaria: 3.1.4.3/3.1.4.3. Número de cromosomas (2n) = 24. Las hembras presentan cuatro pares de mamas.</t>
         </is>
       </c>
@@ -753,6 +883,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>Tiene el tamaño de un gato doméstico, de cuerpo alargado y esbelto, con extremidades cortas y una cola gruesa tan larga como la longitud de la cabeza más el cuerpo. El pelaje es de color pardo grisáceo con muchas motas oscuras que tienden a alinearse longitudinalmente. En el centro del dorso las manchas llegan a formar una banda continua de pelos oscuros eréctiles que va desde la cruz hasta la base de la cola. En la cola presenta ocho o diez anillos oscuros. El hocico es afilado y blancuzco con una amplia mancha oscura a cada lado. Orejas grandes, manos y pies con cinco dedos provistos de uñas semirretráctiles. Las hembras poseen dos pares de mamas abdominales. Los machos tienden a ser mayores y más pesados que las hembras pero las diferencias entre los individuos adultos no son significativas. CC: 43,2-55,2 cm; C: 33,1-48,5 cm; P: 8,0-9,0 cm; Ps: 1,55-2,25 kg. La subespecie de Ibiza es más pequeña, su peso no supera los 1,3 kg. En Europa G. genetta no se confunde con ninguna otra especie, pero en África es fácil confundirla con otras ginetas, en especial con Genetta tigrina y Genetta maculata. Fórmula dentaria: 3.1.4.2/3.1.4.2. Número de cromosomas (2n) = 54.</t>
         </is>
       </c>
@@ -765,6 +900,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>Es un glírido de aspecto robusto, con orejas bien visibles y larga cola cubierta por una voluminosa capa de pelo. Pelaje gris plateado en el dorso y cola. Los ejemplares adultos presentan frecuentemente pelos negros que le dan tonos sombríos, o a veces con tintes rojizos. En los jóvenes el dorso es de color gris plateado uniforme. Las partes inferiores son blancas o blanco-amarillentas. Los ojos están rodeados por una orla fina de color negro. Medidas corporales, CC: 130,0-190,0 mm; C: 110,0-150,0 mm; P: 25,032,0 mm; O: 15,7-21,0 mm; Ps: 70,0-185,0 g. Las hembras presentan seis pares de mamas: dos pectorales, dos abdominales y dos inguinales. Fórmula dentaria: 1.0.1.3/1.0.1.3. Número de cromosomas (2n) = 62.</t>
         </is>
       </c>
@@ -777,6 +917,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>Es un carnívoro de cuerpo alargado con coloración agutí uniforme. Pelos caracterizados por estar anillados alternativamente de crema claro y pardo-castaño muy oscuro. Cola ancha en la base y estrecha en la punta terminada en mechón negro. Medidas corporales, CC: 46,0-54,0 cm; C: 36,0-45,0 cm; CR: 20,0-27,0 cm; P: 85,0-97,0 mm; O: 2,9-3,6 cm; Ps: 2,0-3,7 kg. Extremidades proporcionalmente muy cortas, con manos y pies de cinco dedos, plantas desnudas y uñas no retráctiles. Cabeza puntiaguda con hocico terminado en un rinario desnudo oscuro. Ojos pequeños con pupilas ovales alargadas horizontalmente. Orejas redondeadas, anchas y cortas. Cráneo estrecho, alto y alargado, con rostro más bien corto, estrecho y obtuso, y caja cerebral larga. Fórmula dentaria: 3.1.4.2/3.1.4.2. Poseen una bolsa glandular desnuda rodeando el ano, en la que se abren glándulas anales, y tres pares de mamas ventrales. Los machos son significativamente más grandes que las hembras tanto en las medidas corporales como en las craneales. No obstante el solapamiento entre las medidas de ambos sexos es grande. Número de cromosomas (2n) = 43 (machos) y 44 (hembras).</t>
         </is>
       </c>
@@ -789,6 +934,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>Murciélago de pequeño tamaño. Orejas cortas, separadas en su base y más anchas y redondeadas que en Pipistrellus; el trago es corto y redondeado, con el extremo ensanchado y dirigido hacia el interior. Pelaje bastante largo; las partes inferiores son normalmente blanco-grisáceas, en ocasiones con tonos amarillentos, mientras que los pelos del dorso son generalmente bicolores, con la base pardo-negruzca y la punta castaña, a menudo con tonos dorados, aunque se ha señalado que pueden ser enteramente oscuros hasta en un 25% de los individuos. Partes desnudas de la piel de color pardo oscuro o negruzco. Plagiopatagio insertado en la base de los dedos y uropatagio con un estrecho epiblema en el espolón. Las últimas dos vértebras (3-5 mm) sobresalen del uropatagio. ANT: 31,6-37,5 mm; Ps: 5,010,0 g. Las hembras son algo mayores que los machos. Fórmula dentaria: 2.1.2.3/3.1.2.3; el I1 es bicúspide y el P1 está desplazado hacia el interior, oculto entre C y P2 en vista lateral y muy reducido, o incluso ausente. Número de cromosomas (2n) = 44. Puede confundirse morfológicamente con Pipistrellus pipistrellus, Pipistrellus kuhlii y Pipistrellus nathusii.</t>
         </is>
       </c>
@@ -801,6 +951,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>Es un roedor plantígrado de gran tamaño, con ojos pequeños y con la espalda parcialmente cubierta de púas. Medidas corporales, CC: 57-68 cm; C: 5-12 cm; P: 7,5-9,5 cm; Ps: 10-30 kg. En la parte posterior del cuerpo y en los cuartos traseros presenta unas largas púas de 30 a 40 cm de longitud, situadas entre otras más cortas y gruesas, con bandas de color blanco y negro. Las hembras poseen de dos a tres pares de mamas torácicas. Fórmula dentaria 1.0.1.3/1.0.1.3.</t>
         </is>
       </c>
@@ -813,6 +968,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>Es algo más grande que el ratón de campo (Apodemus sylvaticus), con la cola un poco más larga que la cabeza y el cuerpo. El pelo de las partes superiores es de color canela claro, a lo largo del dorso corre una lista negra y a cada lado de ésta, en los flancos, hay otras cinco listas negras más anchas que encierran otra línea media de color algo más pálido que el fondo del pelaje. En la zona ventral, el color se degrada hasta el blanco, igual que en los cuatro pies. Medidas corporales, CC: 99,3-108,0 mm; C: 80,0-113,0 mm; O: 12,7-16,0 mm; P: 25,0-28,5 mm; Ps: 38,4-43,0 g. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 54.</t>
         </is>
       </c>
@@ -825,6 +985,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>Presenta un tamaño intermedio entre el de la liebre ibérica (Lepus granatensis) y el de la europea (Lepus europaeus). Medidas corporales, CC: 49,0-51,2 cm; C: 7,8-9,6 cm; P: 13,5-14,4 cm; O: 9,1-9,5 cm; Ps: 2,60-3,45 kg. El color del pelaje es pardo amarillento, con una mayor extensión de la zona blanca ventral que en la liebre europea, llegando en ocasiones a las extremidades anteriores aunque no de forma tan extensa como en la liebre ibérica. El contraste entre el color del dorso y del vientre es nítido, a diferencia de la transición difuminada existente en la liebre europea. Presenta una franja clara distintiva en la cara, entre los ojos y la parte inferior de las mejillas.</t>
         </is>
       </c>
@@ -837,6 +1002,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>Es la mayor de las liebres presentes en la Península Ibérica. Medidas corporales, CC: 49,4-55,8 cm; C: 8,4-9,8 cm; P: 13,8-14,6 cm; O: 9,7-11,3 cm; Ps: 3,0-4,4 kg. Las hembras son algo más pesadas que los machos y aparte de una ligera diferencia de tamaño, no existe dimorfismo sexual por lo que la determinación del sexo sólo puede realizarse por observación de los genitales externos. Las extremidades y orejas son largas, y estas últimas presentan el extremo de color negro. El color del pelo es pardo amarillento, a excepción de la zona ventral en la que es de color blanquecino y de poca extensión. En invierno adquiere tonalidades más grisáceas. La cola es blanca y negra. Fórmula dentaria: 2.0.3.3/1.0.2.3. Es posible confundirla con la liebre ibérica Lepus granatensis y con la liebre de piornal Lepus castroviejoi, aunque difiere de ambas por su mayor tamaño, la menor extensión de la zona clara ventral y la transición progresiva entre el colorido de dorso y vientre.</t>
         </is>
       </c>
@@ -849,6 +1019,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>Es la más pequeña de las liebres españolas. Al igual que sus congéneres presentan unas extremidades posteriores muy desarrolladas y unas orejas muy largas y con los extremos negros. El pelaje es pardo amarillento en su parte dorsal y blanco por  la ventral, destacan las extremidades con una mancha blanca en su parte posterior. Medidas corporales, CC: 44,4-47,0 cm; C: 9,5-10,9 cm; O: 9,6-10,1 cm; P: 11,4-11,8 mm; Ps: 2,06-2,54 kg. Se ha citado un peso máximos de 2,95 kg para los machos y de 3,30 kg para las hembras.</t>
         </is>
       </c>
@@ -861,6 +1036,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>De tamaño semejante al de la liebre ibérica (Lepus granatensis). El color del pelaje del dorso varía entre ante rosado y negro, la borra es de color gris pálido y un círculo blanquecino rodea los ojos. Las orejas son bastante oscuras en su parte externa, con una mancha grande de color negra en la porción distal. No son raros los ejemplares que presentan una pequeña mancha blanca en la frente. La nuca presenta una gran mancha de color canela. Las zonas laterales son de color avellana y el vientre blanco. Cola negra por el dorso y blanca por los laterales y la parte ventral. Medidas corporales, CC: 46,550,0 cm; C: 6,0-9,5 cm; O: 10,0-10,5 cm; P: 11,5-12,8 cm.</t>
         </is>
       </c>
@@ -873,6 +1053,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>Mustélido de cuerpo alargado y extremidades proporcionalmente cortas. La cabeza es ancha y aplanada, sin que se aprecie un cuello diferenciado. Ojos, oídos y orificios nasales se encuentran desplazados hacia la parte superior de la cabeza. La cola es ancha y aplanada en la base, y puntiaguda en el extremo. Posee cinco dedos unidos por una membrana interdigital bien desarrollada, tanto en las extremidades anteriores como en las posteriores. El pelaje es de color castaño o pardo con diversas tonalidades; en la garganta y parte superior del pecho destaca una mancha bien representada, de color más claro. Presenta vibrisas largas en hocico, boca, mentón, ojos y antebrazos. El dimorfismo sexual es acusado. Medidas corporales de ejemplares adultos, CC: 60,4-75,0 cm (machos), 59,0-71,0 cm (hembras); C: 39,0-49,0 cm (machos), 35,9-45,0 cm (hembras); Ps: 6,1-9,4 kg (machos), 4,4-6,5 kg (hembras). Fórmula dentaria: 3.1.4.1/3.1.3.2. Número de cromosomas (2n) = 38. Los adultos no pueden ser confundidos con ninguna otra especie, salvo con el visón europeo, Mustela lutreola, visón americano, Neovison vison y el turón, Mustela putorius, habitantes también de ríos y masas de agua, pero con un tamaño mucho menor.</t>
         </is>
       </c>
@@ -885,6 +1070,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>Aspecto estilizado, con extremidades largas, cabeza relativamente pequeña y cola corta. Cráneo con frente alta y rostro corto. Fórmula dentaria: 3.1.2.1/3.1.2.1. Pelaje de la cabeza, dorso, flancos y exterior de las patas de color leonado salpicado de manchas oscuras de tamaño variable. Unos mechones de pelos largos (patillas) flanquean los lados de la cara y las orejas puntiagudas acaban en pinceles negros, el mismo color de la punta de la cola. Presenta cuatro pares de mamas abdominales; el par anterior se suele desarrollar poco y apenas se detecta. Medidas corporales de individuos adultos de Doñana: CC: 74,7-87,5 cm (machos), 69,0-78,5 cm (hembras); C: 12,6-16,9 cm (machos), 11,0-16,7 cm (hembras); CR: 41,0-55,0 cm (machos), 36,0-47,0 cm (hembras); P: 17,0-20,0 cm (machos), 15,518,5 cm (hembras); Ps: 7,5-15,9 kg (machos), 6,1-12,4 kg (hembras). Número de cromosomas (2n) = 38.</t>
         </is>
       </c>
@@ -897,6 +1087,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>Es un roedor de gran tamaño. Cabeza y orejas cortas. Extremidades anteriores fuertes con cuatro dedos y adaptadas a la excavación. Cinco dedos en las extremidades posteriores. Medidas corporales, CC: 50-60 cm; C: 15 cm; Ps: 3,4-5,7 kg. Las hembras presentan de cuatro a cinco pares de mamas abdominales y torácicas. Adulto con cabeza y espalda de color pardo oscuro, nariz grisácea y vientre amarillo. Tercio distal de la cola negro o muy oscuro. Crías hasta los tres meses de color gris. Tienen una sola muda anual, entre junio y agosto, en la que muestran abundante alopecia en forma de calvas. Dimorfismo sexual apreciable sólo por la distancia ano-genital (machos: 4,0-4,8 cm; hembras: 1,7-2,2 cm), o las mamas conspicuas durante la lactancia. Fórmula dentaria: 1.0.2.3/1.0.1.3. Número de cromosomas (2n) = 38.</t>
         </is>
       </c>
@@ -909,6 +1104,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>Presenta el aspecto característico de un mustélido adaptado al medio arborícola, con el cuerpo alargado, cabeza estrecha y morro afilado, ojos y orejas relativamente grandes, extremidades cortas, cola larga y muy peluda. Presenta un enorme parecido externo con la marta, Martes martes, aunque su pelo es más castaño y la borra más blanquecina que la de ésta. Tan sólo se pueden distinguir con seguridad por el color del babero, ocre o anaranjado en la marta y blanco en la garduña. El cráneo de ambas especies es casi idéntico y los caracteres diagnósticos no son constantes, por lo que se requiere cierta experiencia para distinguir ambas especies. Presenta un marcado dimorfismo sexual. Medidas corporales, CC: 420-530 mm (machos), 380-460 mm (hembras); C: 200-290 mm (machos), 170-230 mm (hembras); P: 33-50 mm (machos), 35-48 mm (hembras); Ps: 1.100 -2.500 g (machos), 900-1.400 g (hembras). Las hembras tienen dos pares de mamas. Número de cromosomas (2n) = 38.</t>
         </is>
       </c>
@@ -921,6 +1121,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>Mustélido de tamaño medio, de cuerpo alargado y extremidades cortas. No presenta dimorfismo sexual. Pelaje de color castaño oscuro uniforme, muy tupido y adaptado a las condiciones de frío extremo donde suele vivir. Destaca de su pelaje la presencia abundante de pelos entre los dedos que le permiten caminar sobre la nieve blanda y dibujan una huella típica difuminada. Mancha típica de color ocre o anaranjado en la zona de la garganta que casi siempre suele ocupar sólo una pequeña porción de la mandíbula inferior. La garduña, Martes foina, es la única especie con la que podría llegar a confundirse en España, excepto por el color y la forma de la mancha pectoral blanca que llega en casi todos los casos a ocupar el principio de las extremidades anteriores. Medidas corporales, CC: 513–659 mm (machos), 465–572 mm (hembras); Ps: 800-1.600 g (machos), 750-1.200 g (hembras). En el cráneo presenta una cresta sagital, más marcada en los machos. Fórmula dentaria: 3.1.4.1/3.1.4.2. Número de cromosomas (2n) = 38.</t>
         </is>
       </c>
@@ -933,6 +1138,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>Es un mustélido de gran tamaño, robusto, con cabeza pequeña, cuello ancho y corto, cuerpo alargado, cola y extremidades cortas y uñas largas y resistentes. La cabeza es de color blanco con dos bandas negras que cubren los ojos, el cuerpo es de color gris en la parte dorsal y más oscuro en la ventral. El dimorfismo sexual es reducido, especialmente en el sur de la Península. Las medidas de ejemplares adultos de Doñana son las siguientes, CC: 58,2-75,0 cm; C: 11,4-20,0 cm; P: 8,8-12,0 cm. El peso es variable y depende del sexo, la disponibilidad de alimento y la estación del año, en Doñana se alcanzan valores de 5,9-9,3 kg (machos) y 4,8-9,2 kg (hembras). En el norte peninsular los individuos son ligeramente más pesados y de mayor tamaño. No hay confusión posible con otras especies. Fórmula dentaria: 3.1.4.1/3.1.4.2. Número de cromosomas (2n) = 44.</t>
         </is>
       </c>
@@ -945,6 +1155,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>Es el múrido más pequeño, con un rostro breve, hocico romo y orejas redondas, que destacan entre el pelaje. La cola es prensil, característica de un animal trepador. Color similar al de otros múridos silvestres: castaño rojizo en la parte dorsal (de tonalidad más grisácea en los individuos juveniles) y blanco en la parte ventral. Medidas corporales, CC: 48,0-75,0 mm; C: 39,0-65,0 mm; P: 12,0-15,0 mm; Ps: 6,0-15,0 g. Cráneo pequeño y corto, con serie molar superior que rara vez alcanza los 3,0 mm. Fórmula dentaria: 1.0.0.3/1.0.0.3. M1 con cinco raíces (tres en Mus y cuatro en Apodemus) y mandíbula con siete alvéolos (seis en Apodemus y cinco en Mus). Puede ser confundido con ejemplares jóvenes de Apodemus o de Mus (especialmente con el ratón moruno, Mus spretus, pero no presenta muesca en el I1). Número de cromosomas (2n) = 68.</t>
         </is>
       </c>
@@ -957,6 +1172,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>Es un arvicolino de tamaño mediano y de aspecto robusto. Hocico bastante romo y cola relativamente corta. Aunque las orejas están más cubiertas por el pelo, externamente presenta una morfología muy similar a la del topillo campesino, Microtus arvalis, del que puede llegar a ser difícil de distinguir. Medidas corporales, CC: 95,0-123,0 mm; C: 25,0-44,5 mm; P: 16,0-21,0 mm; O: 10,0-13,5 mm; Ps: 21,0-41,4 g. El pelaje es pardo grisáceo en el dorso con los flancos más pálidos, que pueden llegar a ser amarillentos. La garganta, el vientre y las patas son grises, a veces cremosos en los individuos adultos. La cola presenta una coloración más oscura en su parte dorsal. La textura del pelaje varía con las estaciones, siendo más fino durante el período invernal. Los jóvenes son más grises y oscuros que los adultos. Presentan seis almohadillas plantares en los pies y cuatro pares de mamas, dos pectorales y dos inguinales. Las apófisis coronoidea y articular forman un ángulo más abierto que en M. arvalis. Dientes de crecimiento continuo y raíz abierta. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 50.</t>
         </is>
       </c>
@@ -969,6 +1189,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>Pequeño arvicolino de aspecto macizo y redondeado. Cola y orejas cortas. La subespecie M. a. asturianus, que habita en la mitad norte de la Península, es de mayor tamaño (CC: 67,0-144,0 mm; C: 18,049,0 mm; P: 15,0-21,0 mm; O: 6,0-15,0 mm; Ps: 17,5-72,0 g) que M. a. arvalis que aparece en el Pirineo (CC: 96,0-122,0 mm; C: 28,0-42,0 mm; P: 15,0-18,0 mm; O: 11,0-14,0 mm; Ps: 18,0-41,0 g). El pelaje de los adultos es pardo-amarillento en el dorso y blanco grisáceo en el vientre. Los jóvenes presentan una coloración general grisácea. Sin dimorfismo sexual en cuanto a tamaño o coloración. Las hembras presentan cuatro pares de mamas: dos pectorales y dos inguinales. El cráneo es corto y ancho, los arcos zigomáticos sobresalen notablemente y las bulas timpánicas son pequeñas. La mandíbula es fuerte y presenta un engrosamiento en su parte posterior provocado por la raíz del incisivo. Los dientes son de crecimiento continuo y de raíz abierta. Fórmula dentaria: 1.0.0.3/1.0.0.3. Morfológicamente es muy semejante al topillo agreste, Microtus agrestis y externamente sólo es posible diferenciarlos observando el borde exterior de la oreja, que está cubierto por el pelo en el caso del topillo agreste y es claramente visible en el topillo campesino. La dentición ofrece otro rasgo diferenciador: el M2 del topillo agreste presenta un lóbulo en la parte posterior interna del diente que no se aprecia en el topillo campesino. Número de cromosomas (2n) = 46.</t>
         </is>
       </c>
@@ -981,6 +1206,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>Es un arvicolino robusto que se encuentra entre los de mayor tamaño de su género. Medidas corporales, CC: 116,0-130,0 mm; C: 33,0-46,0 mm; P: 20,0-22,0 mm; O: 13,0-16,0 mm; Ps: 40,0-68,0 g. No existe dimorfismo sexual en las medidas corporales ni craneales, aunque ambos sexos presentan diferencias en las dimensiones de la pelvis. El pelaje es largo y espeso, de color pardo o gris oliváceo en el dorso y de color crema sucio en la región ventral. Los pies son parduscos con los dedos blanquecinos y la cola es gris pardusca por encima y amarillenta por debajo. Los individuos juveniles tienen un pelaje más uniforme, de color grisáceo en el dorso y región ventral. Poseen cuatro pares de mamas, dos pectorales y dos inguinales. En cuanto a la morfología craneal, se caracteriza por el perfil superior convexo, huesos nasales más largos que el diastema y anchos posteriormente (estos dos rasgos diferencian al topillo de Cabrera de otras especies de topillos), mandíbula muy robusta con apófisis digástrica muy desarrollada, I1 tan ancho en norma frontal como en norma lateral, M2 con cuatro prismas y M3 formado por tres prismas y sin ningún triángulo cerrado, gran desarrollo de los forámenes incisivo y timpánico y foramen mandibular desplazado hacia el borde posterior. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 54.</t>
         </is>
       </c>
@@ -993,6 +1223,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>Es un arvicolino de pequeño tamaño, aunque algo más robusto que el topillo lusitano, Microtus lusitanicus. Medidas corporales de ejemplares del sur de la Península Ibérica, CC: 80,0-110,0 mm; C: 23,035,0 mm; P: 14,5-18,5 mm; O: 7,5-10,0 mm; Ps: 19,0-32,0 g. Los hábitos subterráneos se hacen patentes en la reducción de los ojos, las orejas y en la presencia de pelos cortos y flexibles. El pelaje es de un tono pardo amarillento, aunque las tonalidades claras y oscuras varían según el área de distribución. Es característica la aparición en los flancos de una banda ocre muy marcada que hace muy evidente la separación entre el dorso y el vientre. La cola es de color gris homogéneo, a diferencia de la de M. lusitanicus en el que siempre es bicolor. Presenta además incisivos superiores más prominentes y un mayor desarrollo del premaxilar, y por lo tanto también del diastema. Los arcos zigomáticos son muy fuertes y prominentes. Molares hipsodontos, de crecimiento continuo y raíz abierta. Fórmula dentaria: 1.0.0.3/1.0.0.3. Presenta dos pares de mamas inguinales. Número de cromosomas (2n) = 62.</t>
         </is>
       </c>
@@ -1005,6 +1240,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>Es un arvicolino de pequeño tamaño, con el cuerpo alargado y las extremidades y cola proporcionalmente cortas. El hocico es corto y romo y los ojos relativamente pequeños en comparación con los restantes Microtus que no pertenecen al subgénero Pitymys. Las orejas son también pequeñas y están inmersas en el pelaje, más que en el M. duodecimcostatus. Todas estas características denotan su adaptación a la vida subterránea y naturaleza cavadora. Medidas corporales, CC: 94,0-104,5 mm; C: 27,5-34,0 mm; P: 15,0-16,0 mm; O: 7,5-8,5 mm; Ps: 18,0-24,0 g. La coloración del pelaje es parda, más rojiza en el dorso y grisácea en el vientre. La cola es bicolor, con la parte dorsal oscura y la ventral clara. Presentan dos pares de mamas inguinales. El cráneo es pequeño y de aspecto frágil, sin caracteres diferenciales de valor sistemático. Las piezas dentales son hipsodontas, de crecimiento continuo y raíz abierta. En la mandíbula inferior, los incisivos son largos pero no provocan ningún ensanchamiento notable en la parte posterior de la mandíbula. En el M1, por delante del bucle posterior, se encuentran tres triángulos cerrados y los dos siguientes (también anteriores al bucle) están ampliamente en contacto conformando lo que se denomina “triángulo pitimiano”, característico de los topillos del subgénero Pitymys. M. gerbei y M. duodecimcostatus, en el Pirineo occidental, se pueden diferenciar mediante un análisis discriminante basado en medidas mandibulares. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 54. 415 Catalán: Talpó pirinenc l Eusquera: Satain piriniarra l Gallego: Alemán: Pyrenäen-Kleinwühlmaus l Francés: Campagnol des Pyrénées l Inglés: Pyrenean pine vole l Portugués: Orden Rodentia l  Suborden Myomorpha l  Familia Cricetidae l  Subfamilia Arvicolinae ESPECIE AUTÓCTONA Topillo pirenaico Microtus gerbei (Gerbe, 1879)</t>
         </is>
       </c>
@@ -1017,6 +1257,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>Es un arvicolino de pequeño tamaño, de orejas y cola cortas. Medidas corporales, CC: 77,5-105,0 mm; C: 17,0-30,0 mm; O: 6,5-10,0 mm; P: 13-16 mm; Ps: 14,0-19,0 g. La forma del cuerpo refleja su vida de tipo subterráneo: cabeza grande, hocico romo, ojos pequeños y cuerpo cilíndrico. Boca pequeña con incisivos superiores que se proyectan muy ligeramente. La coloración general del dorso varía del gris oscuro al sepia, a veces con reflejos ocres en los flancos. Vientre completamente gris. Cola bicolor, con dorso más oscuro. No se ha descrito dimorfismo en la coloración pero los juveniles son de un gris más oscuro que los adultos. Presenta dos pares de mamas en posición inguinal. El perfil dorsal del cráneo es moderadamente convexo. La caja craneana es alta y redondeada. Los cóndilos son visibles en vista dorsal porque la zona posterior de la caja craneana es menos angulosa que en el topillo mediterráneo Microtus duodecimcostatus. La región interorbital es ancha y aplastada. En los individuos más adultos los bordes posteriores se extienden escasamente hacia atrás por la región parietal. Las bulas auditivas son pequeñas y redondeadas. Fórmula dentaria: 1.0.0.3/1.0.0.3. Dientes molariformes con raíces abiertas toda la vida y que decrecen en tamaño hacia la zona posterior. Segundo triángulo externo del tercer molar superior muy reducido y sin alcanzar la altura del primero y tercero. Número de cromosomas (2n) = 62.</t>
         </is>
       </c>
@@ -1029,6 +1274,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>Es un murciélago de mediano tamaño, con hocico muy corto, perfil achatado y frente alta y protuberante. Las orejas son pequeñas y triangulares, con un trago corto, redondeado y proyectado hacia dentro. Las alas son largas y estrechas, con la segunda falange del tercer dedo muy larga, tres veces la longitud de la primera. El plagiopatagio se inserta a la altura del tobillo y el uropatagio carece de lóbulo poscalcáneo. Pelaje corto y denso, de color pardo grisáceo en el dorso y más pálido en la zona ventral y formado por pelos  más oscuros en su mitad basal. ANT: 42,9-49,9 mm; Ps: 10,1-20,8 g. Fórmula dentaria: 2.1.2.3/3.1.3.3. Número de cromosomas (2n) = 46. No es preciso su examen en mano para su correcta identificación.</t>
         </is>
       </c>
@@ -1041,6 +1291,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>Es un múrido de pequeño tamaño, con hocico redondeado y ojos y orejas pequeños. Medidas corporales de ejemplares adultos del sur de la Península, CC: 75,0-93,5 mm; C: 60,0-76,5 mm; P: 16,018,0 mm; O: 11,0-14,0 mm; Ps: 12,0-21,0 g. Los adultos presentan una coloración dorsal gris castaño, con una franja cefalocaudal más oscura. Vientre blanco grisáceo, con una nítida línea de separación lateral entre ambas regiones corporales. Pelaje juvenil algo más oscuro que el de adulto. Se diferencia fácilmente del ratón casero Mus musculus, por su coloración y por la longitud relativa de la cola, que es siempre bastante menor que la del cuerpo. Su coloración es bastante parecida a la de los juveniles del ratón de campo Apodemus sylvaticus, pero se diferencia de ellos por presentar unos ojos y orejas mucho menores y una longitud del pie posterior siempre inferior a 18 mm. Las hembras presentan cinco pares de mamas: tres pectorales y dos inguinales. Cráneo más corto y redondeado que el de M. musculus, del que se diferencia fácilmente por la mayor anchura de la rama dorsal del arco zigomático y un perfil más redondeado de la placa zigomática. Fórmula dentaria: 1.0.0.3/ 1.0.0.3. Dientes muy parecidos a los de M. musculus, pero con cuatro lóbulos bien diferenciados en la región anterior del M1. Número de cromosomas (2n) = 40.</t>
         </is>
       </c>
@@ -1053,6 +1308,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>Es un pequeño mustélido, algunas formas son las más pequeñas de los carnívoros. Cuerpo alargado con extremidades cortas, cuello largo y cabeza aplanada, orejas cortas y redondeadas. La cola representa el 37% de la longitud corporal, su último tercio termina en pincel y es de color negro. El colorido del pelaje es pardo rojizo en el dorso y laterales, y blanco en el vientre. Presenta librea invernal completamente blanca, excepto el extremo de la cola. Cuando está con librea estival podría confundirse con la comadreja (Mustela nivalis) en zonas de simpatría. Posee un gran dimorfismo sexual reflejado en la talla, siendo las hembras hasta un 40% más pequeñas que los machos. Medidas externas para la subespecie centroeuropea, M. erminea aestiva, CC: 244-278 mm (machos), 221-250 mm (hembras); C: 92-124 mm (machos), 70-100 mm (hembras); O: 41-52 mm (machos), 37-49 mm (hembras); P: 18-27 mm (machos), 17-25 mm (hembras); Ps: 180-330 g (machos), 110-205 g (hembras). Fórmula dentaria 3.1.3.1/3.1.3.2. Presentan cinco o seis pares de mamas. Número de cromosomas (2n) = 44.</t>
         </is>
       </c>
@@ -1065,6 +1325,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>Es un pequeño mustélido adaptado a la vida semiacuática. Su pelaje es corto, de color castaño “chocolate” uniforme y contorno de los labios (tanto inferior como superior) de un distintivo color blanco. Las orejas apenas sobresalen del pelo y presentan membranas interdigitales incompletas en manos y pies. Muestra un acusado dimorfismo sexual en el tamaño. En España, los machos pesan casi un 70% y miden (LT) un 15% más que las hembras. Medidas corporales, LT: 500-800 mm (machos), 430-505 mm (hembras); CC: 305-430 mm (machos), 309-350 mm (hembras); C: 130-185 mm (machos), 130156 mm (hembras); P: 54-82 mm (machos), 50-60 mm (hembras); Ps: 700-1.100 g (machos), 450650 g (hembras). Las hembras presentan habitualmente tres pares de mamas. En el campo puede confundirse con el turón Mustela putorius, pero éste presenta un antifaz blanco en la cara y una estrecha mancha blanca en el borde de las orejas. Es casi idéntico al visón americano Neovison vison, si bien éste es algo mayor y no presenta el labio superior blanco. Fórmula dentaria: 3.1.3.1/3.1.3.2. Número de cromosomas (2n) = 38.</t>
         </is>
       </c>
@@ -1077,6 +1342,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>Es el mustélido más pequeño, de cuerpo y cabeza alargados y extremidades cortas. Cola corta, aproximadamente el 30% del cuerpo. Pelaje de color pardo canela a pardo chocolate en la parte dorsal, y blanco en la ventral, con el límite entre coloraciones recto o sinuoso según las formas descritas. Los pies, con 5 dedos, pueden ser blancos o con la coloración dorsal. En la cara presentan con frecuencia pecas rictales. Acusado dimorfismo sexual en la longitud corporal (los machos son un 10-20% más largos que las hembras). La longitud también varía a lo largo de su distribución. Medidas corporales de ejemplares adultos de la Península Ibérica, CC:175-250 mm (machos), 165-190 mm (hembras); C: 50-85 mm (machos), 40-55 mm (hembras); P: 27-37 mm (machos), 23-27 mm (hembras); Ps: 90-223 g (machos), 49-80 g (hembras). Fórmula dentaria 3.1.3.1/3.1.3.2. Número de cromosomas (2n) = 42. Las hembras presentan cuatro pares de mamas. Podría confundirse con el armiño en librea estival, aunque no posee el tercio apical negro en la cola, ni presenta en estas latitudes librea blanca invernal. 283 Catalán: Mustela l Eusquera: Erbinudea l Gallego: Denociña Alemán: Mauswiesel l Francés: Belette l Inglés: Weasel l Portugués: Doninha Orden Carnivora l Suborden Caniformia l  Familia Mustelidae  l  Subfamilia Mustelinae ESPECIE AUTÓCTONA Comadreja Mustela nivalis Linnaeus, 1766</t>
         </is>
       </c>
@@ -1089,6 +1359,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>Mustélido de tamaño intermedio entre la marta, Martes martes y el armiño, Mustela erminea. El cuerpo es esbelto y alargado. Medidas corporales, CC: 385-425 mm; C: 150 mm; Ps: 800-1.300 g (machos), en hembras es un 60-90% inferior. La coloración general es bastante uniforme, normalmente tostado oscuro, pero se aclara en ambos flancos. Presenta un característico antifaz blanco alrededor del hocico y las regiones auriculares y oculares. El dimorfismo sexual es bastante marcado, aunque sin llegar al caso de la comadreja, Mustela nivalis, o el armiño, M. erminea. Fórmula dentaria: 3.1.3.1/3.1.3.2. Número de cromosomas (2n) = 40.</t>
         </is>
       </c>
@@ -1101,6 +1376,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>Su aspecto general es el de una gran rata con un largo rabo desnudo y cilíndrico. Posee diversas adaptaciones a la vida semiacuática: extremidades posteriores palmeadas; orejas pequeñas; ojos y orificios nasales situados en la parte dorsal de la cabeza, lo que les permite ver y oler mientras nadan; labios que se pueden cerrar por detrás de los incisivos. Cinco dedos en manos y pies. Incisivos anaranjados siempre visibles. Los machos son mayores que las hembras. Medidas corporales de ejemplares del Reino Unido (valores medios), CC: 60,3 cm (machos), 59,3 cm (hembras); Ps: 6,5 kg (machos), 6,0 kg (hembras). Pelaje con pelos de jarra de color pardo, más denso en el dorso, y con algunas jarras amarillentas. Pelo de borra grisáceo. Vibrisas, extremo del hocico y mejillas blancas. Las hembras tienen cuatro pares de mamas inguinales (a veces cinco). Huellas de las extremidades de hasta 15 cm de longitud, con membrana interdigital visible. Arrastran la cola por el barro. Excrementos cilíndricos (70 x 11 mm), estriados longitudinalmente y pardos. Cráneo con amplio foramen infra-orbital y arco zigomático robusto. Formula dentaria: 1.0.1.3/1.0.1.3. Los incisivos son más anchos en los machos que en las hembras. Número de cromosomas (2n) = 42. No se puede confundir con ninguna otra especie silvestre de la Península Ibérica. No se han llevado a cabo estudios de cierta entidad sobre la especie en España.</t>
         </is>
       </c>
@@ -1113,6 +1393,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>Se trata de un Myotis de tamaño mediano, destacando el tamaño de sus orejas anchas y largas. El borde externo de la oreja presenta nueve pliegues transversales. El trago es largo y tiene forma de lanceta. El pelaje es largo con la base del pelo pardo oscuro y de color gris claro la cara ventral. Las crías presentan un color gris claro. Presenta un espolón recto con una longitud aproximada de entre un tercio y la mitad de la del uropatagio, estando la última vértebra caudal libre. El plagiopatagio empieza en la base de los dedos. Puede presentar albinismo parcial. ANT: 39,0-47,0 mm; O: 23,0-26,0 mm; Ps: 7,0-14,0 g. Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Se diferencia de los Myotis del mismo tamaño por la mayor longitud de sus orejas y de los Plecotus, por tener las orejas separadas en su base, por lo que no es necesario su captura para una correcta identificación.</t>
         </is>
       </c>
@@ -1125,6 +1410,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>En el 95% de los ejemplares destaca la presencia de una mancha blanca en el pelaje frontal. ANT: 50,5-62,0 mm; Ps: 18,0-29,5 g. Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n)= 44. Semejante a M. myotis y M. punicus, aunque más esbelto y con un hocico más fino. Puede confundirse con M. myotis si carece de la mancha blanca. Para diferenciarlos se estudia la relación entre las longitudes del antebrazo y la oreja (Z = 0,433ANT + 3,709O), completando el análisis con la de la serie dental superior (M. blythii: Z &lt; -0,3; CM3 &lt; 9 mm; M. myotis: Z &gt; 0,3; CM3 &gt; 9 mm), aunque no siempre es posible.</t>
         </is>
       </c>
@@ -1137,6 +1427,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>Es un murciélago de tamaño mediano. No se ha descrito dimorfismo sexual. La coloración del pelaje dorsal es gris clara, siendo el pelaje ventral casi blanco. El pie, que presenta cerdas, es conspicuamente grande, mayor que la mitad de la tibia. La tibia presenta, característicamente, una densa cubierta de pelos, que se extiende por las zonas próximas del patagio. Los jóvenes presentan habitualmente una mancha oscura en el mentón. ANT: 38,2-44,6 mm; Ps: 5,5-15,0 g. (Levante y Baleares). Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Puede ser confundido con Myotis daubentonii, siendo el mejor criterio para distinguirlos la ausencia de pelo abundante en la tibia en este último.</t>
         </is>
       </c>
@@ -1149,6 +1444,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>Murciélago de pequeño tamaño. El dorso es de color pardo rojizo a negruzco y el vientre blanco sucio. Pelo bicolor, con la base oscura, especialmente en la zona ventral. Las orejas, relativamente cortas, apenas llegan al extremo del hocico si se pliegan hacia delante. El plagiopatagio se inserta en la mitad del pie, que es bastante largo y ancho. Tibia sin pilosidad aparente. El espolón ocupa dos terceras partes del borde del uropatagio, que está desnudo o con escasos pelos. Existen numerosas citas de casos de albinismo. Juveniles gris oscuro y con una mancha negra en el labio inferior. ANT: 33,2-38,7 mm; Ps: 7,0-15,0 g. Puede encontrarse o no protocónulo en P4. Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Es necesaria su identificación en mano al poder confundirse con otras especies pequeñas del género Myotis, como M. nattereri, M. emarginatus o M. mystacinus.</t>
         </is>
       </c>
@@ -1161,6 +1461,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>Murciélago de tamaño mediano-pequeño, con orejas de longitud media que extendidas llegan justo hasta el hocico. Presentan una escotadura en la oreja más marcada que en otras especies. Trago puntiagudo que apenas alcanza dicha escotadura. Pelaje de aspecto lanoso rubio rojizo dorsalmente y amarillento ventralmente. El plagiopatagio se inserta en la base del dedo más externo del pie. El espolón ocupa la mitad del borde posterior del uropatagio, que generalmente presenta algunos pelos pequeños. La tibia está parcialmente cubierta de pelos rojizos en su parte dorsal. Jóvenes más oscuros sin tonos rojizos. ANT: 37,8-39,7 mm (machos), 39,9-42,6 mm (hembras); Ps: 7,4-10,0 g (machos), 8,511,5 g (hembras) (datos de Navarra). Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosoma (2n) = 44. Se puede confundir con otros Myotis de tamaño pequeño: M. nattereri, M. bechsteinii, M. daubentonii y M. capaccinii.</t>
         </is>
       </c>
@@ -1173,6 +1478,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>Es el mayor Myotis de Europa. Las hembras algo mayores que los machos. Pelo corto y denso, de base oscura, con dorso castaño a pardo grisáceo y vientre casi blanco; los jóvenes gris cenicientos. Piel pardo rojiza. Hocico ancho y con abultamientos glandulares. Uropatagio lampiño, con un espolón que cubre la mitad de su borde. ANT: 56,5-62,3 mm; Ps: 21,0-35,0 gr. Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Se confunde con Myotis blythii cuando éste no presenta su frecuente mancha blanca frontal, en cuyo caso es necesario realizar un análisis biométrico.</t>
         </is>
       </c>
@@ -1185,6 +1495,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>Rostro, orejas y membranas alares pardo negruzcas. La oreja extendida hacia delante supera ligeramente el extremo del hocico y presenta una muesca marcada de la que sobresale un trago puntiagudo y algo mayor que la mitad de la oreja. Las membranas alares se insertan en la base del dedo más externo del pie. El espolón ocupa la mitad de la distancia del borde del uropatagio entre pie y cola. El pie es pequeño y su longitud es la mitad de la tibia. El pene es delgado y no se engrosa en el extremo. El pelaje es largo, algo encrespado y bicolor, con la base de los pelos pardo negruzca y las puntas más claras. En los adultos, el dorso es castaño dorado y la región ventral varía de crema pálido a blanquecino. Jóvenes más oscuros y grisáceos. Se ha citado la existencia de ejemplares albinos. ANT: 31,5-36,5 mm; Ps: 3,9-8,0 g. En los ejemplares españoles identificados por medio de técnicas moleculares: 33,034,9 mm y 3,9-4,5 g, respectivamente. Ambos sexos son de tamaño similar. En el cráneo, la cúspide palatal del cíngulo del P4 está menos desarrollada que en M. alcathoe, vista desde la parte interna está por debajo del P3. El P3 es claramente menor que el P2, pero algo mayor que su mitad y el P3 es más pequeño que el P2. Formula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Las mayores posibilidades de confusión se dan con sus especies gemelas, M. alcathoe y M. brandtii. La primera es algo menor en sus medidas externas, de forma que por el momento, la longitud del antebrazo de los M. alcathoe españoles es igual o menor a 33,0 mm. El trago es igual que la mitad de la oreja y ésta es más corta y redondeada. El color de las partes desprovistas de pelo es pardo rojizo, salvo la base 176 Catalán: Rat penat de bigotis l Eusquera: Saguzar bibotedun l Gallego: Morcego de bigotes Alemán: Kleine Bartfledermaus l Francés: Murin à moustaches l Inglés: Whiskered bat l Portugués: Morcego-de-bigodes  Orden Chiroptera l  Familia Vespertilionidae ESPECIE AUTÓCTONA Murciélago ratonero bigotudo Myotis mystacinus (Kuhl, 1817) interna de la oreja y la piel que está alrededor del ojo que aparece poco o nada pigmentadas (color rosado). En los adultos, el pelo del dorso es de color pardo oscuro en la base y castaño rojizo en las puntas. En general, M. alcathoe presentaría una morfología muy similar a la de M. mystacinus pero con la librea típica de M. daubentonii. En el cráneo, el cíngulo palatal del P4 está más desarrollado y es del tamaño del P3, que a su vez, es la mitad del P2. Aunque M. brandtii nunca ha sido citado en España, sus principales diferencias morfológicas deberían ser tenidas en cuenta cuando se identifique a M. mystacinus. M. brandtii es algo mayor y tiene el pene engrosado en el extremo. Las cúspides del P4 son del tamaño del P3. El P3 y el P3 son aproximadamente de similar talla que el P2 y el P2, respectivamente. Por el momento, para realizar con seguridad una correcta identificación de los ejemplares de esta especie y de sus gemelas, es imprescindible realizar análisis moleculares comparativos de ADN mitocondrial (están secuenciados de forma completa o parcial los genes citocromo b, ND1 y 12S rRNA). En consecuencia, todos los datos no avalados por este tipo de análisis deberían ser consignados provisionalmente como M. mystacinus s.l. En M. daubentonii el espolón ocupa las dos terceras partes del borde del uropatagio, el ala se inserta en la mitad del pie, que es más grande y presenta en los dedos unos pelos rígidos muy característicos. También se puede confundir con algunos Pipistrellus, pero estos tienen el extremo del trago redondeado y dos premolares superiores.</t>
         </is>
       </c>
@@ -1197,6 +1512,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>Murciélago de tamaño pequeño, con orejas que extendidas sobrepasan el hocico. Presenta una emarginación en la oreja, aunque menos marcada que en M. emarginatus. Trago puntiagudo típico del género. El espolón ocupa la mitad del borde del uropatagio; la otra mitad tiene una conspicua y densa franja de pelos cortos y rígidos. Las tibias carecen de pilosidad aparente. Coloración general grisaceoleonada y el vientre más claro que el dorso, con un fuerte contraste entre ambos. Pelo bicolor, el dorsal con base oscura y puntas pardo-grisáceas y el ventral con base también oscura y puntas blanquecinas. Destaca la falta de pelo alrededor de los ojos. Los jóvenes son mucho más oscuros que los adultos. Ambos sexos son de tamaño similar. ANT: 35,6-41,9 mm; Ps: 6,4-8,5 g (Navarra), 6,6-8,5 g (Andalucía Occidental), 4,9-6,0 g (Menorca). Fórmula dentaria: 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Aspecto general similar a otras especies del mismo género. En mano, sin embargo, la presencia de una conspicua franja de pelos en el borde del uropatagio y el espolón en forma de “S” y sin pelos aparentes son suficientes para distinguirlos.</t>
         </is>
       </c>
@@ -1209,6 +1529,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>Talla grande. Dorso pardo claro con el pelo negruzco en la base y pardo en la punta. Vientre blanco sucio con la punta de los pelos blanquecina. Carece de mancha blanca en la frente. Los jóvenes de color grisáceo. Orejas elípticas, largas (superan el hocico al proyectarse hacia delante), trago lineal con extremo apuntado. Zonas desnudas de la cara de color carne. Membranas sepia con la inserción de las alas en la base del dedo más externo del pie. Espolones sin lóbulo poscalcáneo. ANT: 55,0-63,0 mm; Ps: 20,0-29,5 g. Fórmula dentaria 2.1.3.3/3.1.3.3. Número de cromosomas (2n) = 44. Los nóctulos y el murciélago de huerta tienen las orejas más cortas, trago más ancho y zonas de piel desnuda negruzcas. Los otros murciélagos ratoneros no comparten área de distribución.</t>
         </is>
       </c>
@@ -1221,6 +1546,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>Es un sorícido de tamaño medio. Medidas corporales, CC: 72,0-90,0 mm; C: 52,0-72,0 mm; P: 14,518,0 mm; Ps: 9,0-16,0 g. Externamente es similar al musgaño patiblanco (Neomys fodiens) si bien su tamaño es algo menor y sus adaptaciones al medio acuático menos acentuadas; concretamente, el pie posterior es más pequeño, la quilla de pelos de la cola ocupa como máximo su mitad distal y la densidad de pelos es menor en los márgenes de manos, pies y dedos. Al igual que N. fodiens presenta glándulas que secretan una saliva ligeramente narcotizante. Las hembras presentan de cuatro a seis pares de mamas. El pelaje es prácticamente de color negro en el dorso y gris con reflejos plateados, pardos, rojizos o amarillentos en la región ventral. Pueden existir manchas blancas detrás de los ojos, dibujos negros de diseño e intensidad variables o incluso ejemplares muy melanizados. La cola es bicolor, sepia o negruzca por encima y blanca por debajo. El dorso de los juveniles es más claro que el de los adultos. El cráneo es semejante al de N. fodiens aunque de menor tamaño, más frágil y de perfil más bajo. Para diferenciar biométricamente a N. anomalus de N. fodiens existen diversas fórmulas discriminantes establecidas a partir de parámetros mandibulares. En los ejemplares ibéricos la altura de la apófisis coronoides es generalmente inferior a 4,8 mm (compárese con N. fodiens). Fórmula dentaria: 3.1.2.3/1.1.1.3, con cuatro unicúspides superiores. Cúspides dentarias pigmentadas de rojo. Sus dientes son menos robustos que los de N. fodiens. Número de cromosomas (2n) = 52.</t>
         </is>
       </c>
@@ -1233,6 +1563,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>Es el sorícido ibérico de mayor tamaño. Medidas corporales, CC: 68,0-97,0 mm; C: 53,0-69,0 mm; P: 16,5-19,5 mm; Ps: 10,0-23,0 g. Al ser un animal semiacuático presenta toda una serie de adaptaciones morfológicas a la natación como por ejemplo: tercio posterior del cuerpo ancho, pies relativamente grandes, ribete de pelos rígidos en manos, pies y dedos y cola provista de una hilera medioventral de pelos largos, blancos y rígidos que discurre por toda su longitud (compárese con el musgaño de Cabrera, Neomys anomalus). Presenta glándulas salivales que secretan una sustancia ligeramente narcotizante. El pelaje del dorso es oscuro, casi negro, y la región ventral gris plateada con reflejos pardos, rojizos o negros. La cola es negruzca por encima y blanca por debajo o bien totalmente negra. En algunos animales pueden aparecer manchas blancas sobre el hocico, detrás de los ojos, detrás de los pabellones auditivos o en la base de la cola. El pelaje dorsal de los juveniles es más claro y más pardusco que el de los adultos. Las hembras presentan de cinco a siete pares de mamas. El perfil dorsal del cráneo aumenta de manera acentuada desde el rostro hasta el neurocráneo, existiendo una conspicua elevación rostral a nivel del I1. El contorno posterior del rostro es trapezoidal y la caja craneana es alta, redondeada posteriormente y subcircular. La apófisis condilar de la mandíbula es robusta y con las facetas articulares manifiestamente separadas. Para diferenciar biométricamente a N. fodiens de N. anomalus se han propuesto varias fórmulas discriminantes basadas en variables mandibulares. En los ejemplares ibéricos la altura de la apófisis coronoides es generalmente superior a 4,7 mm (compárese con N. anomalus). Fórmula dentaria: 3.1.2.3/1.1.1.3, con cuatro unicúspides superiores. Cúspides dentarias pigmentadas de rojo. Comparativamente con N. anomalus los dientes son más robustos y los unicúspides superiores más anchos. Número de cromosomas (2n) = 52.</t>
         </is>
       </c>
@@ -1245,6 +1580,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>Es el mayor murciélago europeo. No parece mostrar dimorfismo sexual en tamaño. Pelo monocolor. Pelaje denso, largo y lustroso, que se extiende por el patagio. Dorso de color variable desde castaño a rojizo. Vientre más claro o amarillento. Los jóvenes son mas grisáceos. Orejas cortas, anchas y redondeadas, con el antitrago grueso y el trago grande y de forma arriñonada. Las alas, largas y relativamente estrechas, se insertan en el tobillo. Lóbulo poscalcáneo bien desarrollado. ANT: 61,3-67,8 mm (datos ibéricos). Dentición robusta. Fórmula dentaria: 2.1.2.3/3.1.2.3. Número de cromosomas (2n) = 42. Sólo podría confundirse, por su tamaño, con el murciélago rabudo, Tadarida teniotis, pero éste es grisáceo, de cola libre y alas aún mas estilizadas, y por su morfología, con el nóctulo mediano, Nyctalus noctula, aunque éste es algo más pequeño (antebrazo menor de 60 mm), menos robusto y de orejas menos anchas en su parte superior.</t>
         </is>
       </c>
@@ -1257,6 +1597,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>Rostro, orejas y membranas alares pardo oscuro. Las alas son largas y relativamente estrechas (5º metacarpo mucho menor que 3º y 4º), presentan un denso pelaje en la zona próxima al cuerpo y brazos, y se insertan en el tobillo. Lóbulo poscalcáneo bien desarrollado. Orejas relativamente más cortas y estrechas que en otros nóctulos, el trago tiene forma de riñón. Pelaje corto y bicolor, base de los pelos pardo oscuro y puntas más claras. Dorso castaño y región ventral pardo más claro, a veces con tonos amarillentos. En La Rioja se han capturado varios ejemplares parcialmente albinos. ANT: 39,0-47,0 mm; Ps: 8,0-23,2 g. Las hembras son algo mayores que los machos. Formula dentaria: 2.1.2.3/3.1.2.3. Número de cromosomas (2n) = 46. En los otros nóctulos el P1 no es visible, son de mayor talla y su coloración general es más rojiza. En el resto de las especies de aspecto similar el trago no es arriñonado y la talla es menor.</t>
         </is>
       </c>
@@ -1269,6 +1614,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>Es un murciélago de tamaño grande. Las orejas son anchas, aproximadamente redondeadas; el trago, arriñonado. El hocico es corto y ancho. Las alas son largas y estrechas. Las membranas alares se insertan en los tobillos. Alas, orejas y hocico de color castaño oscuro. El pelaje es pardo-dorado. ANT: 48,0-58,0 mm; Ps: 18,0-40,0 g. Fórmula dentaria: 2.1.2.3/3.1.2.3. Su identificación debe hacerse en mano.</t>
         </is>
       </c>
@@ -1281,6 +1631,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>Al igual que todos los lagomorfos, presenta potentes extremidades traseras adaptadas a la carrera, grandes pabellones auriculares, aunque menores que los del género Lepus, con una coloración uniforme (las liebres presentan una coloración negruzca en la parte distal de las orejas). Su pelaje muestra variaciones en tonalidades pardas y grisáceas, destacando claramente el blanco de la parte interna de la cola, sin una mancha negra tan claramente definida como en Lepus. Medidas corporales, CC: 3435 cm; Ps: 0,90-1,34 kg (O. c. algirus), 1,50-2,00 kg (O. c. cuniculus).</t>
         </is>
       </c>
@@ -1293,6 +1648,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
           <t>Es la forma más pequeña del género Ovis, y presenta un dimorfismo sexual muy pronunciado. Medidas corporales, CC: 127-145 cm (machos), 120-130 cm (hembras); CR: 75-80 cm (machos), 70-75 cm (hembras); Ps: 40-60 kg (machos), 30-40 kg (hembras). En los machos la variedad en la forma de los cuernos es muy acusada. En el caso de las hembras, entre el 12 y el 60% presentan cuernos que se consideran residuales y que rara vez alcanzan los 15 cm. El pelo es de color castaño oscuro, aunque hay individuos de color más claro (tipo cremoso). Como peculiaridades presentan una serie de manchas blancas, en forma de silla de montar, en los lomos, la región (escudo) anal está bien marcada, así como la cara, con un área blanquecina encima del morro y debajo del frontal que va aumentando con la edad, hasta ocupar toda la cara. El vientre y la parte interior de las extremidades son blancos. Los caracteres mas relevantes que los diferencian del género Capra son la cola larga cubierta de pelos, ausencia de mechón de pelos en la barbilla y cráneo muy convexo, además de otras características osteométricas diferenciales. Número de cromosomas (2n) = 54. El número actual de cromosomas deriva de los ancestros comunes de los Ovis con NF = 60. El número cromosómico del muflón es similar al de la oveja doméstica y al de Ovis orientalis. También es similar al de los pachiceros. 371 Catalán: Mufló l Eusquera: Mufloia l Gallego: Alemán: Mufflon l Francés: Moufflon l Inglés: Moufflon, Wild sheep l Portugués: Muflon Orden Artiodactyla l  Familia Bovidae ESPECIE ALÓCTONA Muflón Ovis aries Linnaeus, 1758</t>
         </is>
       </c>
@@ -1305,6 +1665,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>Es un murciélago pequeño. Las orejas son cortas, triangulares y con vértice superior redondeado, y poseen cinco pliegues transversales en la parte superior del borde externo. El trago es corto, redondeado en la punta y ligeramente curvado. El pelaje es de coloración general pardo castaño o rojizo en la parte dorsal, y más claro en la zona ventral. El hocico, las orejas y la membrana alar son de color negro parduzco. Las alas son relativamente estrechas. El plagiopatagio se inserta en la base de los dedos del pie; en su borde presentan generalmente una banda de color más claro. El espolón alcanza más de la mitad de la longitud del borde del uropatagio, con lóbulo postcalcáneo con cartílago conspicuo en forma de T. Los incisivos internos superiores (I1) son monocúspides, los externos (I2) menores que la mitad del I1, y el premolar superior anterior (P1) está desplazado hacia el interior y no es visible externamente. Los incisivos inferiores están fuertemente imbricados, y no presentan diastema entre I2 e I3. ANT: 31,0-37,0 mm; Ps: 4,5-10,0 g. Fórmula dentaria: 2.1.2.3/3.1.2.3. Número de cromosomas (2n) = 44. No existe dimorfismo sexual, aunque las hembras son algo mayores. Puede confundirse sobre todo con los otros representantes del género Pipistrellus y en menor medida con Hypsugo savii, de los que se diferencia sobre todo por los caracteres dentales.</t>
         </is>
       </c>
@@ -1317,6 +1682,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
           <t>Murciélago de pequeño tamaño y muy parecido a Pipistrellus kuhlii, del que casi con toda seguridad se ha originado. Coloración general pardo madera, piel desnuda más oscura que su pariente cercano. El pequeño premolar superior siempre es visible desde el exterior, al contrario que ocurre en Pipistrellus kuhlii. Borde claro en la parte posterior de la membrana alar casi siempre hasta el 5º dedo; en los ejemplares de Madeira esta característica está ausente y en los de La Palma sólo está presente en una parte de la población. ANT: 29,9-34,9 mm; Ps: 2,9-5,7 g. Las hembras son mayores que los machos. Par de incisivos superiores externos unicúspides, en ocasiones sin sobresalir de la encía. Fórmula dentaria: 2.1.2.3/3.1.2.3. Número de cromosomas desconocido.</t>
         </is>
       </c>
@@ -1329,6 +1699,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t>El pelaje dorsal de los adultos es de color pardo rojizo durante el verano y pardo oscuro con tonos grises durante el invierno. El vientre es pardo claro o amarillento. Los juveniles tienen el dorso pardo oscuro, careciendo de los tonos grises del pelaje invernal de los adultos. Superficie dorsal del uropatagio cubierta de pelo al menos hasta la mitad. Como en los otros Pipistrellus, las orejas son cortas y el trago es un poco más largo que ancho y de punta redondeada. No se dispone de información sobre dimorfismo sexual. ANT: 32,0-37,0 mm; Ps: 6,0-15,5. Fórmula dentaria: 2.1.2.3/3.1.2.3. Los caninos son grandes, especialmente los inferiores, cuya anchura antero-posterior supera la mitad de su altura. El P1 es claramente visible y está alineado exteriormente con el resto de los dientes. El I2 es mayor que la longitud de la segunda cúspide del I1. Los incisivos inferiores no están imbricados y existe un diastema entre I2 e I3. Número de cromosomas (2n) = 44. Puede confundirse con las otras especies del mismo género. El color de Hypsugo savii es muy diferente. En cualquier caso, la identificación es sencilla utilizando los caracteres dentarios indicados.</t>
         </is>
       </c>
@@ -1341,6 +1716,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
           <t>Es el murciélago más pequeño de Europa (ANT: 28,8-32,8 mm; Ps: 4,1-7,5 g) . Orejas cortas y triangulares. Trago de punta redondeada, más largo que ancho. Pelaje dorsal desde marrón-oliva a arenoso pálido. La región ventral es más clara. La razón entre la longitud de la 2ª y 3ª falange del 3er dedo es 1:1, aunque este carácter es bastante variable. Las orejas y el hocico son relativamente más cortos y el pelaje dorsal del uropatagio más denso y extendido que en el murciélago enano, cubriéndolo hasta su tercio proximal. La pigmentación de las partes desnudas de la cara presenta parches claros conspicuos. En los machos el pene es anaranjado y sin la estría distintiva del murciélago enano. Ambos sexos presentan una pequeña protuberancia entre los orificios nasales, ausente en su especie gemela . Fórmula dentaria: 2.1.2.3/3.1.2.3. Forma y disposición de los incisivos superiores y PM1 como en el murciélago enano. Se distingue con relativa facilidad de otros miembros del mismo género por su tamaño menor y su morfología dentaria.</t>
         </is>
       </c>
@@ -1353,6 +1733,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
           <t>Es el murciélago más pequeño de Europa (ANT: 28,8-32,8 mm; Ps: 4,1-7,5 g) . Orejas cortas y triangulares. Trago de punta redondeada, más largo que ancho. Pelaje dorsal desde marrón-oliva a arenoso pálido. La región ventral es más clara. La razón entre la longitud de la 2ª y 3ª falange del 3er dedo es 1:1, aunque este carácter es bastante variable. Las orejas y el hocico son relativamente más cortos y el pelaje dorsal del uropatagio más denso y extendido que en el murciélago enano, cubriéndolo hasta su tercio proximal. La pigmentación de las partes desnudas de la cara presenta parches claros conspicuos. En los machos el pene es anaranjado y sin la estría distintiva del murciélago enano. Ambos sexos presentan una pequeña protuberancia entre los orificios nasales, ausente en su especie gemela . Fórmula dentaria: 2.1.2.3/3.1.2.3. Forma y disposición de los incisivos superiores y PM1 como en el murciélago enano. Se distingue con relativa facilidad de otros miembros del mismo género por su tamaño menor y su morfología dentaria.</t>
         </is>
       </c>
@@ -1365,6 +1750,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
           <t>Murciélago de talla media. Orejas muy largas, membranosas y unidas en la base donde se localiza un proceso en forma de botón. Trago con el borde interno prácticamente recto y de color blanco amarillento que resulta casi translúcido. Pulgar largo, cuya uña generalmente sobrepasa los 2 mm de longitud. Plagiopatagio inserto en la base de los pies. Las hembras son significativamente mayores en varios caracteres externos (antebrazo, pulgar, quinto dedo, trago, y pie). El pelaje es abundante, largo y denso de coloración parda amarillenta o parda grisácea en el dorso, aunque su parte basal es claramente parda. En su parte ventral la coloración es gris claro con tintes amarillentos. Los individuos juveniles tienen un color más pálido, sin tintes pardos y su cara es más oscura. ANT: 36,9-43,5 mm; Ps: 6,8-12,0 g. Fórmula dentaria: 2.1.2.3/3.1.3.3. Número de cromosomas (2n) = 32. Las dos especies de orejudos son bastante difíciles de diferenciar y solamente es posible hacerlo en mano.</t>
         </is>
       </c>
@@ -1377,6 +1767,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
           <t>Es un murciélago de tamaño medio. Orejas muy grandes que se unen por la base de sus bordes internos. El dorso es gris oscuro con los pelos negruzcos en casi toda su longitud, mientras que la zona ventral es blanquecina o gris muy pálida. Los jóvenes tienen una coloración grisácea más apagada. Las hembras son por lo general algo mayores que los machos. ANT: 37,0-45,0 mm; Ps: 6,5-15 g. Fórmula dentaria:  2.1.2.3/3.1.3.3. Número de cromosomas (2n) = 32. Por el tamaño de las orejas y su aspecto, en la Península Ibérica sólo se puede confundir con P. auritus y la semejanza entre ambas requiere que su determinación deba realizarse en mano, y aún así pueden surgir dificultades. Al contrario que en P. auritus, el trago es normalmente mayor de 5,5 mm y está pigmentado en toda su longitud con un color parecido al del pabellón de la oreja. La longitud del pulgar (sin la uña) generalmente es menor (inferior a 6 mm) y la uña es también más corta. Partes desnudas de color grisáceo oscuro (y no pardas o rojizas). Antifaz oscuro alrededor de los ojos más marcado. En los machos adultos, el pene es mazudo (y no cilíndrico).</t>
         </is>
       </c>
@@ -1389,6 +1784,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
           <t>Murciélago de mediano tamaño, muy parecido a Plecotus austriacus, con coloración general más oscura que éste y de mayor tamaño. Los jóvenes son más oscuros que los adultos. Orejas de aproximadamente 40 mm. ANT: 40,1-46,0 mm; Ps: 6,4-9,1 g. Las hembras son mayores que los machos. Número de cromosomas desconocido. Fórmula dentaria: 2.1.2.3/3.1.3.3.</t>
         </is>
       </c>
@@ -1401,6 +1801,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
           <t>Mucho mayor que la rata negra Rattus rattus, presenta un hocico redondeado, ojos relativamente más pequeños y orejas que al ser estiradas nunca alcanzan el borde del ojo. Medidas corporales de ejemplares silvestres de Cataluña, CC: 172,0-262,0 mm; C: 149,0-222,0 mm; P: 37,0-46,0 mm; O: 16,022,0 mm; Ps: 180,0-415,0 g. Los ejemplares de medios urbanos alcanzan dimensiones mayores y las hembras son ligeramente más pequeñas que los machos. Los juveniles presentan una coloración homogénea gris oscura, mientras que los adultos son algo más claros, con una coloración dorsal gris pardusca y el vientre de amarillento a gris sucio. Se diferencia fácilmente de R. rattus por su coloración y por la longitud relativa de la cola, que es siempre bastante menor que la del cuerpo. Las hembras poseen seis pares de mamas: tres pectorales y tres inguinales. El cráneo es fuerte y la caja craneana más estrecha que en R. rattus, con crestas temporales y occipitales poco marcadas y que discurren casi paralelas, lo que confiere al cráneo un aspecto casi rectangular. La mandíbula presenta una hendidura posterior de perfil ovalado. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 42.</t>
         </is>
       </c>
@@ -1413,6 +1818,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
           <t>Es un múrido de cuerpo alargado, hocico puntiagudo y largas orejas que alcanzan el borde del ojo al estirarse hacia delante. Medidas corporales de ejemplares adultos del sur de la Península, CC: 158,0232,0 mm; C:181,0-247,0 mm; P: 31,0-39,5 mm; O: 20,0-26,5 mm; Ps: 87,0-278,0 g. Las hembras son ligeramente más pequeñas que los machos. Los adultos presentan una coloración dorsal muy oscura, con tonos que varían desde el gris oscuro, casi negro, en el morfotipo rattus hasta el pardo rojizo de frugivorus y alexandrinus. El vientre es siempre más claro, desde el gris de rattus y frugivorus hasta el blanco amarillento de alexandrinus. La línea de separación no está muy bien definida pero es visible. Se diferencia fácilmente de la rata parda Rattus norvegicus, por su coloración y por la longitud relativa de la cola, que es siempre bastante mayor que la del cuerpo. Las hembras poseen cinco pares de mamas: dos pectorales y tres inguinales. Cráneo más corto y ovalado que el de R. norvegicus, con arcos zigomáticos menos sobresalientes y crestas temporales y occipitales con un diseño curvo característico. La mandíbula presenta una hendidura posterior con un perfil en el que la zona angular es más corta. Fórmula dentaria: 1.0.0.3/1.0.0.3. Número de cromosomas (2n) = 38 (tipo europeo) y 42 (tipo asiático).</t>
         </is>
       </c>
@@ -1425,6 +1835,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
           <t>Es un rinolofo de tamaño medio. La coloración dorsal es gris parda más clara en la base, y la ventral blanco grisácea o ligeramente amarillenta. Las membranas alares y orejas son de color gris pardo claro. Los jóvenes presentan una coloración más clara. La proyección conectiva superior de la silla es afilada y ligeramente curvada hacia abajo, netamente más larga que la inferior; la arista entre ambas proyecciones presenta un perfil lateral claramente cóncavo. Los bordes de la silla son paralelos y la forma de la lanceta se aproxima a un triángulo equilátero. ANT: 44,0-50,5 mm; Ps: 7,2-16,0 g. Fórmula dentaria: 1.1.2.3/2.1.3.3. Número de cromosomas (2n) = 58. En la Península Ibérica puede confundirse con R. mehelyi, del que se distingue mediante examen en mano por su menor tamaño de antebrazo, y por las características de las excrecencias nasales. Una longitud de antebrazo inferior a 48,9 mm corresponde a R. euryale con una fiabilidad del 90%.</t>
         </is>
       </c>
@@ -1437,6 +1852,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
           <t>Es el representante del género Rhinolophus de mayor tamaño en la Península Ibérica. La hoja o lanceta generalmente es ancha y corta, y aguzada hacia la punta. La proyección conectiva en vista lateral es alargada y redondeada. El labio inferior presenta un surco vertical en el centro. Sus orejas son grandes, antitrago ancho y separado del borde externo por una escotadura poco profunda. El plagiopatagio está inserto por debajo del tobillo. El uropatagio se encuentra sostenido por espolones poco desarrollados, y con ausencia de lóbulos postcalcáneos. Las hembras presentan un par de mamas pectorales y un par de falsas mamas inguinales. El pelaje es largo, suave y denso y no se extiende sobre la superficie dorsal de las membranas, las cuales son de color pardo negruzco y semitransparentes. El color de la parte dorsal del cuerpo es pardo oscuro y la parte ventral es mucho más pálida. Los individuos jóvenes son mucho más claros y grises que los adultos. ANT: 50,5-60,2 mm; Ps: 14,6-31,6 g. Fórmula dentaria: 1.1.2.3/2.1.3.3. Número de cromosomas (2n) = 58. Resulta difícil de confundir con el resto de sus congéneres, por lo que no es necesario examinarlo en mano para su correcta identificación.</t>
         </is>
       </c>
@@ -1449,6 +1869,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
           <t>Es el más pequeño de los rinolofos de la región Paleártica. Existe dimorfismo sexual ANT: 35,7-39,0 mm (machos), 35,2-37,5 mm (hembras); Ps: 4,2-6,0 g (machos), 3,7-5,0 g (hembras). Orejas grandes. La silla de la excrecencia nasal es estrecha, con los bordes rectos y convergentes hacia arriba, y la proyección conectiva redondeada en la cresta. Patagio inserto en el tobillo. Uropatagio angular. Coloración dorsal parda más o menos oscura, que responde a la punta de los pelos que en su base son de un color gris claro; la parte ventral algo más clara, de coloración grisácea. Las crías tienen un pelaje suave y de color gris oscuro. Orejas y membranas alares siempre más oscuras que el pelo del dorso. En estado de reposo se envuelve totalmente en la membrana alar. Fórmula dentaria: 1.1.2.3/2.1.3.3. Número de cromosomas (2n) = 56.</t>
         </is>
       </c>
@@ -1461,6 +1886,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
           <t>Es un murciélago de tamaño mediano. En esta especie es característica la forma del proceso conectivo de la silla vista de perfil. La hoja es ancha en la base estrechándose bruscamente hacia el segundo tercio de su altura, a partir del cual continúa estrecho hasta la punta. En su coloración típica, presenta un pelaje dorsal gris parduzco contrastado con un pelaje ventral casi blanco. El límite entre pelaje dorsal y ventral está bastante marcado. Alrededor de los ojos, el pelaje es muy oscuro, formando un “antifaz”. En el suroeste peninsular, aparecen con frecuencia ejemplares con una tonalidad anaranjada brillante muy patente. ANT: 47,0-54,0 mm; Ps: 10,0-18,0 g. Fórmula dentaria: 1.1.2.3/2.1.3.3. Número de cromosomas (2n) = 58. Similar a R. euryale, siendo necesaria su identificación en mano. Se distingue por su mayor tamaño y por las características de las excrecencias nasales.</t>
         </is>
       </c>
@@ -1473,6 +1903,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
           <t>Es un bóvido de pequeño tamaño, menor y más esbelto que la cabra montés Capra pyrenaica. Ambos sexos poseen cuernos en forma de gancho, siendo los de los machos más gruesos y con el gancho apical más cerrado. Cabeza y garganta claras, con una mancha oscura que cubre el ojo a modo de antifaz. Color del cuerpo casi uniforme, con una línea longitudinal más oscura en el dorso. Medidas corporales, CC: 105-120 cm; CR: 70-80 cm; Ps: 20-28 kg. Los machos son algo más pesados que las hembras, aunque las diferencias de peso entre sexos no suelen ser significativas en el rebeco pirenaico y parecen disminuir con el aumento de la densidad y el empobrecimiento del hábitat. Fórmula dentaria: 0.0.3.3/4.0.3.3. Número de cromosomas (2n) = 58.</t>
         </is>
       </c>
@@ -1485,6 +1920,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
           <t>Presenta un aspecto inconfundible, con hocico corto, cuerpo esbelto y larga cola peluda. Tonos rojizos, pardos o negros en el dorso y blanco puro en abdomen, pecho y arranque ventral de las extremidades. Pinceles auriculares sólo desarrollados en invierno. Sin dimorfismo sexual. Los juveniles se reconocen por su menor tamaño y cola poco poblada. Pelaje invernal más denso y oscuro que el estival. Alta variabilidad individual en la extensión de las zonas blancas y en las tonalidades superiores. Medidas corporales de ejemplares de Cataluña, CC: 195,0-247,0 mm; C:140,0-195,0 mm; P: 50,0-68,0 mm; Ps: 203,0-385,0 g. Las ardillas españolas más corpulentas, de dorso vinoso, son las de Sierra Espuña, en Murcia. Fórmula dentaria: 1.0.2.3/1.0.1.3. Las hembras presentan cuatro pares de mamas: uno pectoral, dos abdominales y otro inguinal. Número de cromosomas (2n) = 40.</t>
         </is>
       </c>
@@ -1497,6 +1937,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
           <t>Es un soricino de mediano tamaño, con la longitud de la cola generalmente superior a la de la mitad de la cabeza y cuerpo, CC: 65,0-85,0 mm; C: 40,0-55,0 mm; P: 12,0-14,0 mm; Ps: 6,0-15,0 g. Presenta un hocico largo, acabado en una pequeña trompa provista de vibrisas. Los ojos son pequeños y poco visibles, y las orejas están prácticamente cubiertas por el pelaje. Éste es denso, especialmente en invierno, y bicolor. En general, existe una transición gradual entre las coloraciones dorsal y ventral. Los juveniles y los adultos de verano muestran una tonalidad pardusca, más o menos oscura. En invierno, el pelaje es más largo y oscuro, predominando los tonos grisáceos. Presenta tres pares de mamas inguinales. El cráneo es alargado, con la región craneana bien diferenciada de la región interorbital y de perfil subcircular. La mandíbula es frágil, con la apófisis coronoides recta o ligeramente dirigida hacia atrás y la apófisis articular medianamente desarrollada. La fosa temporal presenta el contorno bastante triangular, con el margen inferior recto. El foramen mandibular, a menudo doble, se sitúa en una depresión poco marcada y se extiende hasta la mitad del borde inferior de la fosa temporal. Fórmula dentaria: 3.1.3.3/1.1.1.3, con cinco unicúspides superiores. Cúspides dentarias pigmentadas de rojo. El incisivo inferior se prolonga siguiendo el eje de la rama horizontal de la mandíbula y el tercer molar inferior no muestra reducción apreciable del talónido. Ciertos caracteres somáticos y craneales, especialmente el peso y la altura de la caja craneana, experimentan una notable reducción invernal (fenómeno Dehnel); dicho fenómeno se interpreta como una adaptación a condiciones ambientales adversas y a la escasa disponibilidad de alimento. Número de cromosomas (2n) = 18-30. La variación en la dotación cromosómica se debe a Fusiones Robertsonianas. Los machos presentan trivalente sexual XY1Y2. Morfológica y morfométricamente la especie apenas difiere de la musaraña tricolor, Sorex coronatus.</t>
         </is>
       </c>
@@ -1509,6 +1954,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
           <t>La musaraña tricolor presenta una morfología corporal similar a la de la musaraña bicolor, pero de dimensiones ligeramente menores, CC: 62,0-76,0 mm; C: 40,0-50,0 mm; P: 11,8-13,7 mm; Ps: 6,513,5 g. Aunque el pelaje muestra una notable variación geográfica, generalmente es tricolor, con el dorso pardo oscuro, los flancos netamente más claros y el vientre pardo grisáceo. En los juveniles y adultos de verano, el dorso y los flancos son más claros y en el vientre predominan tonos parduscos. Las hembras presentan tres pares de mamas inguinales. El cráneo es también parecido al de S. araneus, pero con la mandíbula más robusta, la apófisis coronoides generalmente inclinada hacia delante y la apófisis articular más desarrollada y dirigida hacia atrás. La fosa temporal interna presenta el contorno inferior ovoide y el foramen mandibular, habitualmente simple, se sitúa bajo la mitad posterior de dicha fosa, en una depresión bien marcada. Fórmula dentaria: 3.1.3.3/1.1.1.3, con cinco unicúspides superiores. Cúspides dentarias pigmentadas de rojo. A diferencia de S. araneus, el incisivo inferior está ligeramente dirigido hacia arriba y el tercer molar presenta reducción perceptible del talónido. Número de cromosomas (2n) = 20. Los machos presentan trivalente sexual XY1Y2. Morfológica y morfométricamente, la especie puede confundirse con S. araneus y S. granarius. Se han propuesto diversas fórmulas discriminantes, basadas en parámetros craneales o mandibulares, para realizar la diferenciación específica, aunque sólo mediante análisis bioquímicos o genéticos es posible una diagnosis inequívoca.</t>
         </is>
       </c>
@@ -1521,6 +1971,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
           <t>La musaraña ibérica es morfológicamente muy semejante a las musarañas bicolor (Sorex araneus) y tricolor (Sorex coronatus), pero presenta unas dimensiones más reducidas, CC: 50,0-72,0 mm; C: 36,046,0 mm; P: 11,0-12,5 mm; Ps: 4,5-8,0 g. El pelaje es similar al de S. coronatus, aunque el dorso carece de banda mediodorsal oscura y el vientre es gris amarillento. Los juveniles muestran una coloración más pálida que los adultos, sin claro contraste entre las regiones dorsal y lateral. Presenta tres pares de mamas inguinales. En comparación con S. araneus y S. coronatus, el cráneo presenta el rostro relativamente más corto, con el paladar ensanchado en la parte anterior. El perfil dorsal de la caja craneana es recto, generalmente sin concavidad evidente en la región interorbitaria. El proceso coronoides de la mandíbula es corto y la apófisis angular delgada. La fosa mandibular es triangular y presenta el ápice dirigido hacia delante. Fórmula dentaria: 3.1.3.3/1.1.1.3, con cinco unicúspides superiores. Cúspides dentarias pigmentadas de rojo aunque generalmente, a diferencia de S. araneus y S. coronatus, los incisivos superiores muestran una tonalidad más clara y los dos primeros molares superiores presentan el hipocono no pigmentado. Número de cromosomas (2n) = 34. Los machos presentan trivalente sexual XY1Y2. S. granarius puede confundirse con S. araneus y S. coronatus. En las zonas en las que aparece en simpatría con la musaraña tricolor, ambas especies pueden diferenciarse mediante la aplicación de diversas fórmulas discriminantes basadas en parámetros craneales, aunque únicamente los análisis genéticos permiten asegurar un diagnóstico específico correcto. Genéticamente la especie está íntimamente emparentada con la musaraña bicolor. En general, se acepta que su cariotipo acrocéntrico representa la forma ancestral del grupo S. araneus-arcticus. Los cariotipos de S. araneus y S. coronatus habrían derivado del de S. granarius a partir de reordenaciones cromosómicas (translocaciones Robertsonianas, translocaciones telómero-centrómero, cambios centroméricos). Contrariamente, estudios de ADN mitocondrial apuntan a S. coronatus como la especie más primitiva del grupo europeo araneus.  108 Catalán: Musaranya ibèrica l Eusquera: Satitsu espainiar l Gallego: Furafollas ibérico Alemán: Iberische Waldspitzmaus l Francés: Musaraigne ibérique l Inglés: Spanish shrew l Portugués: Musaranho-de-dentes-vermelhos Orden Soricomorpha l  Familia Soricidae l  Subfamilia Soricinae ESPECIE AUTÓCTONA l  ENDEMISMO IBÉRICO Musaraña ibérica Sorex granarius Miller, 1910</t>
         </is>
       </c>
@@ -1533,6 +1988,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
           <t>La musaraña enana es el soricino ibérico de menor tamaño, CC: 49,0-72,0 mm; C: 38,0-48,0 mm; P: 10,0-11,5 mm; Ps: 2,7-6,5 g, excepcionalmente hasta 7,5 g. De morfología similar a los restantes representantes del género Sorex, se diferencia de éstos por presentar la cabeza relativamente pequeña, la cola de mayor longitud relativa respecto a la de la cabeza y cuerpo y el pie posterior con una longitud inferior a 12 mm. El pelaje es bicolor, ligeramente más claro y uniforme que en Sorex araneus y S. coronatus. En general, en los pelajes de juvenil y de verano, la coloración dorsal exhibe tonalidades parduscas y la ventral es más o menos gris. El pelaje de invierno es más largo y oscuro, predominando las tonalidades grisáceas, tanto en el dorso como en el vientre. Presenta tres pares de mamas inguinales. El cráneo es también similar al de las demás especies del género, pero de dimensiones más reducidas. La caja craneana muestra el perfil oval y es más baja, estrecha y alargada que en S. araneus. La delimitación entre la región facial y la craneal es poco marcada. La mandíbula es frágil y pequeña, generalmente con una longitud inferior a 9 mm. La apófisis coronoides está claramente dirigida hacia delante y su altura suele ser inferior a 4 mm. Fórmula dentaria: 3.1.3.3/1.1.1.3, con cinco unicúspides superiores. Cúspides dentarias pigmentadas de rojo. A diferencia de S. araneus, el tercer unicúspide superior es igual o mayor que el segundo. El incisivo inferior está provisto de tres lóbulos, notablemente iguales. Como en S. araneus, ciertos parámetros corporales y craneales, especialmente el peso y la altura de la caja craneana, están sometidos a una reducción invernal (fenómeno Dehnel), como adaptación a condiciones ambientales rigurosas y a la escasa disponibilidad de alimento. Número de cromosomas (2n) = 42.</t>
         </is>
       </c>
@@ -1545,6 +2005,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
           <t>Es uno de los mamíferos más pequeños del mundo. Medidas corporales, CC: 35,0-53,0 mm; C: 21,030,0 mm; P: 5,7-7,9 mm; Ps: 1,2-2,7 g. Su morfología externa es similar a la de otras musarañas, pero se distingue por presentar la cabeza proporcionalmente más grande y la cola más larga, de aproximadamente la mitad de la longitud corporal. Las orejas son bien visibles, los ojos pequeños y la cola está revestida de un corto pelaje entre el que sobresalen numerosos pelos dispersos de mayor longitud. La coloración del pelaje muestra pocas variaciones estacionales. En general, es gris pardusca, con ciertos reflejos rojizos en el dorso y de tonalidad más clara en el vientre, sin clara línea de demarcación entre ambas regiones. Presenta tres pares de mamas inguinales. El cráneo es estrecho y alargado, con la caja craneana de perfil superior prácticamente horizontal. La mandíbula es frágil y de dimensiones reducidas. Fórmula dentaria: 3.1.2.3/1.1.1.3. A diferencia del género Crocidura, Suncus se caracteriza por presentar cuatro unicúspides superiores, aunque el último es sumamente pequeño, está desplazado en sentido lingual y queda prácticamente oculto por la cúspide anterior del último premolar. Los dientes de la mandíbula son de morfología similar a los de la musaraña gris, Crocidura russula, aunque de menor tamaño y con la sección posterior del M3 más reducida. Número de cromosomas (2n) = 42.</t>
         </is>
       </c>
@@ -1557,6 +2022,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
           <t>Muestra la máxima altura en la región de las extremidades anteriores; el cuello es poco aparente, las orejas son pequeñas y se mantienen erguidas. Las dimensiones son muy variables; en Europa la corpulencia aumenta hacia el este, observándose los menores tamaños en el sur de la Península Ibérica y los mayores en los Cárpatos. Medidas corporales de ejemplares adultos del Montseny (Cataluña), CC: 133,0-148,0 cm (machos), 118,0-137,0 cm (hembras); C: 17,5-24,0 cm (machos), 13,0-20,0 cm (hembras); CR: 72,0-85,5 cm (machos), 71,0-73,0 cm (hembras); Ps: 60-118 kg (machos), 40-65 kg (hembras). Fórmula dentaria: 3.1.4.3/3.1.4.3. Caninos de puntas agudas y ángulos cortantes. Posee un marcado dimorfismo sexual, los machos son más corpulentos y presentan los caninos más desarrollados. Al nacer, y hasta los cuatro o cinco meses, se denominan rayones y presentan una coloración pardo clara con 11 líneas longitudinales más oscuras. Posteriormente mudan pasando a tener una coloración uniforme pardo rojiza y se denominan bermejos, hasta la siguiente muda que ocurre entre los 10 y 12 meses, cuando adquieren el pelaje de adultos, que es pardo grisáceo, con extremidades y orejas más oscuras, prácticamente negras. La especie muestra politipismo cromosómico. Número de comosomas (2n) = 38, 37 ó 36.</t>
         </is>
       </c>
@@ -1569,6 +2039,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
           <t>Murciélago de gran tamaño, con alas largas y estrechas. Cabeza característica con orejas rígidas proyectadas hacia delante. La cola sobresale por fuera de la membrana caudal y se retrae en el uropatagio en vuelo. El color del pelo es muy variable, de pardo a gris claro. Algunos ejemplares presentan áreas canosas. No se ha descrito dimorfismo sexual en cuanto al color. Las hembras son ligeramente más grandes. ANT: 57,0-64,0 mm; Ps: 22,0-54,0 g. Fórmula dentaria: 1.1.2.3/3.1.2.3. Número de cromosomas (2n) = 48. No existen especies similares en Europa.</t>
         </is>
       </c>
@@ -1581,6 +2056,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
           <t>Externamente el topo europeo es una especie plenamente adaptada a la vida subterránea. Su estructura general es cilíndrica y compacta, con el hocico no muy afilado y la cola corta. Los salientes más destacados del cuerpo son sus extremidades delanteras, con la parte superior dirigida hacia delante, las manos muy ensanchadas y las uñas grandes y aplanadas, teniendo el conjunto la forma de una pala adaptada para excavar. Carece de orejas y los ojos están muy reducidos. El pelaje es muy suave y dispuesto perpendicularmente al cuerpo. Son generalmente de color negro intenso con matices amarillentos en garganta y pecho, pero pueden aparecer ejemplares grises o manchados de amarillo. El topo europeo es algo mayor que el topo ibérico, Talpa occidentalis, con el hocico algo más largo y las patas delanteras relativamente más estrechas. Medidas corporales, CC: 125,0-165,0 mm; C: 25,0-36,0 mm; P: 18,0-21,0 mm; Ps: 72,0-120,0 g. Las hembras tienen cuatro pares de mamas, dos inguinales y dos pectorales. El cráneo es alargado y aplanado, presentando arcos zigomáticos delgados, y la dentición es completa, sin reducciones. Fórmula dentaria: 3.1.4.3/3.1.4.3. Número de cromosomas (2n) = 34. La determinación correcta de la especie sólo debe hacerse a partir de medidas craneales y del uso de caracteres dentarios, como la presencia de un mesostilo simple en los molares superiores.</t>
         </is>
       </c>
@@ -1593,6 +2073,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
           <t>Por la similitud existente entre las dos especies de topos presentes en la Península Ibérica, la descripción dada para el topo europeo es aplicable también al topo ibérico. Como diferencias externas, aunque sin demasiada validez diagnóstica, se puede indicar que el topo ibérico es generalmente más pequeño, con el hocico algo más corto, los ojos siempre ocultos bajo la piel y las extremidades anteriores relativamente más anchas. Medidas corporales, CC: 96,0-130,0 mm; C: 19,0-35,0 mm; P: 14,0-18,0 mm; Ps: 34,0-66,0 g. Fórmula dentaria: 3.1.4.3/3.1.4.3. Número de cromosomas (2n) = 34. La determinación correcta de la especie sólo debe hacerse a partir de medidas craneales y del uso de caracteres dentarios, como la presencia de un mesostilo doble en los molares superiores.</t>
         </is>
       </c>
@@ -1605,6 +2090,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
           <t>De orejas pequeñas y cola corta, el oso pardo se caracteriza por su gran tamaño, cabeza masiva, extremidades cortas y robustas, hombros prominentes y caminar plantígrado. Los machos son más pesados que las hembras. En la Cordillera Cantábrica y Pirineos, las hembras adultas pesan de 75 a 140 kg (un caso excepcional de 245 kg) y los machos de 90 a 250 kg (un caso excepcional de 350 kg). Las manos y pies están provistos de cinco dedos con uñas largas, especialmente las anteriores. El color del pelo varía desde el amarillo pálido hasta el pardo-negruzco y son usuales los contrastes en cabeza, cuello y extremidades (éstas son frecuentemente más oscuras). Las crías suelen presentar un collar claro del que pueden quedar rastros en los adultos. Las hembras tienen tres pares de mamas, pectorales y abdominales. Fórmula dentaria: 3.1.3.2/3.1.2.3.3. Número de cromosomas (2n) = 37.</t>
         </is>
       </c>
@@ -1616,6 +2106,11 @@
         </is>
       </c>
       <c r="B99" t="inlineStr">
+        <is>
+          <t>Inventario IEET - Mamíferos</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
         <is>
           <t>Su larga cola, 70% de la longitud del cuerpo, así como el hocico alargado y las orejas prominentes lo hacen fácilmente reconocible. Sus extremidades son alargadas, con pies más bien pequeños. Los ojos son pequeños y la pupila es vertical. El pelaje es relativamente variable, desde formas casi melánicas hasta ejemplares de coloración pálido-amarillenta. Los zorreznos nacen con un pelaje uniforme pardo oscuro, pero al mes de vida las zonas ventrales de cabeza y tronco, así como las caras mediales de las extremidades, adquieren coloración blanca, mientras los extremos (orejas, morro, pies y manos) permanecen negros y la cola suele tener una banda terminal de pelos blancos, aunque este carácter es inconstante. Presenta una importante variación individual y geográfica en el tamaño. Medidas corporales. CC: 65,0-80,0 cm (machos), 52,0-72,0 cm (hembras); C: 33,0-48,0 cm (machos), 32,0-44,0 cm (hembras); PP: 15,7 cm (machos), 14,5 cm (hembras); Ps: 4,6-8,6 kg (machos), 3,1-7,8 kg (hembras). Fórmula dentaria: 3.1.4.2/3.1.4.3. Número de cromosomas: (2n) = 34.</t>
         </is>

</xml_diff>